<commit_message>
Auto-committed on 2022/04/13 週三
</commit_message>
<xml_diff>
--- a/Program/Other/LM042_底稿_RBC表_會計部_共三份.xlsx
+++ b/Program/Other/LM042_底稿_RBC表_會計部_共三份.xlsx
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="106">
   <si>
     <t>一、非利害關係人放款</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -497,10 +497,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -924,10 +920,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>折溢價及催收費用</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
     <t>應收利息</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
@@ -970,6 +962,22 @@
   <si>
     <t>(空白)</t>
     <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>折溢價與費用</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>放款折溢價</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>催收折溢價及費用</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>利關人金額</t>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3519,7 +3527,7 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="241">
+  <cellXfs count="242">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -4166,6 +4174,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="80" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="188">
@@ -5896,10 +5907,10 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26:C26"/>
+      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
@@ -5920,7 +5931,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="33.5">
       <c r="A1" s="207" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="207"/>
       <c r="C1" s="207"/>
@@ -5936,7 +5947,7 @@
     </row>
     <row r="2" spans="1:12" ht="17">
       <c r="A2" s="221" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" s="221"/>
       <c r="C2" s="221"/>
@@ -5948,7 +5959,7 @@
       <c r="I2" s="221"/>
       <c r="J2" s="221"/>
       <c r="K2" s="59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L2" s="58"/>
     </row>
@@ -5964,32 +5975,32 @@
       <c r="I3" s="222"/>
       <c r="J3" s="222"/>
       <c r="K3" s="60" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L3" s="58"/>
     </row>
     <row r="4" spans="1:12" ht="20.149999999999999" customHeight="1" thickBot="1">
       <c r="A4" s="208" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="209"/>
       <c r="C4" s="212" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="214" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4" s="214"/>
       <c r="F4" s="217" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G4" s="218"/>
       <c r="H4" s="219" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I4" s="220"/>
       <c r="J4" s="215" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K4" s="216"/>
       <c r="L4" s="58"/>
@@ -5999,37 +6010,37 @@
       <c r="B5" s="211"/>
       <c r="C5" s="213"/>
       <c r="D5" s="61" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="62" t="s">
-        <v>29</v>
-      </c>
       <c r="F5" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="62" t="s">
-        <v>29</v>
-      </c>
       <c r="H5" s="64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I5" s="65" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K5" s="67" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L5" s="58"/>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
       <c r="A6" s="223" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="68" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="69"/>
       <c r="D6" s="70"/>
@@ -6045,7 +6056,7 @@
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="A7" s="224"/>
       <c r="B7" s="75" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="76">
         <v>7.1999999999999998E-3</v>
@@ -6081,7 +6092,7 @@
     <row r="8" spans="1:12" ht="30" customHeight="1">
       <c r="A8" s="224"/>
       <c r="B8" s="75" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="76">
         <v>1.0800000000000001E-2</v>
@@ -6117,7 +6128,7 @@
     <row r="9" spans="1:12" ht="30" customHeight="1">
       <c r="A9" s="224"/>
       <c r="B9" s="75" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="76">
         <v>3.9600000000000003E-2</v>
@@ -6153,7 +6164,7 @@
     <row r="10" spans="1:12" ht="30" customHeight="1">
       <c r="A10" s="224"/>
       <c r="B10" s="75" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="76">
         <v>4.7999999999999996E-3</v>
@@ -6189,7 +6200,7 @@
     <row r="11" spans="1:12" ht="30" customHeight="1">
       <c r="A11" s="224"/>
       <c r="B11" s="83" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="84"/>
       <c r="D11" s="85">
@@ -6229,7 +6240,7 @@
     <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="A12" s="224"/>
       <c r="B12" s="68" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="84"/>
       <c r="D12" s="87"/>
@@ -6245,7 +6256,7 @@
     <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="A13" s="224"/>
       <c r="B13" s="92" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="84"/>
       <c r="D13" s="93" t="s">
@@ -6273,7 +6284,7 @@
     <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="224"/>
       <c r="B14" s="92" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="76">
         <v>0.23710000000000001</v>
@@ -6309,7 +6320,7 @@
     <row r="15" spans="1:12" ht="28.9" customHeight="1">
       <c r="A15" s="224"/>
       <c r="B15" s="83" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="84"/>
       <c r="D15" s="85">
@@ -6349,7 +6360,7 @@
     <row r="16" spans="1:12" ht="34.5" customHeight="1" thickBot="1">
       <c r="A16" s="225"/>
       <c r="B16" s="98" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="99"/>
       <c r="D16" s="100">
@@ -6388,10 +6399,10 @@
     </row>
     <row r="17" spans="1:12" ht="33.75" customHeight="1" thickTop="1">
       <c r="A17" s="226" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="103" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="104"/>
       <c r="D17" s="105">
@@ -6431,7 +6442,7 @@
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="227"/>
       <c r="B18" s="68" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="76"/>
       <c r="D18" s="85"/>
@@ -6447,7 +6458,7 @@
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="227"/>
       <c r="B19" s="92" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="76">
         <v>7.1999999999999998E-3</v>
@@ -6483,7 +6494,7 @@
     <row r="20" spans="1:12" ht="30" customHeight="1">
       <c r="A20" s="227"/>
       <c r="B20" s="83" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="76"/>
       <c r="D20" s="85">
@@ -6523,7 +6534,7 @@
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="227"/>
       <c r="B21" s="68" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="76"/>
       <c r="D21" s="85"/>
@@ -6539,7 +6550,7 @@
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="227"/>
       <c r="B22" s="92" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="76"/>
       <c r="D22" s="109">
@@ -6573,7 +6584,7 @@
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="227"/>
       <c r="B23" s="92" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="76">
         <v>0.23710000000000001</v>
@@ -6609,7 +6620,7 @@
     <row r="24" spans="1:12" ht="30" customHeight="1" thickBot="1">
       <c r="A24" s="113"/>
       <c r="B24" s="114" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="99"/>
       <c r="D24" s="205">
@@ -6686,7 +6697,7 @@
     </row>
     <row r="26" spans="1:12" s="8" customFormat="1" ht="27.75" customHeight="1">
       <c r="A26" s="117" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B26" s="117"/>
       <c r="C26" s="118"/>
@@ -6702,7 +6713,7 @@
     </row>
     <row r="27" spans="1:12" s="6" customFormat="1" ht="17">
       <c r="A27" s="121" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27" s="122"/>
       <c r="C27" s="123"/>
@@ -6763,15 +6774,15 @@
         <v>19</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C31" s="17"/>
       <c r="D31" s="12"/>
       <c r="E31" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H31" s="11" t="s">
         <v>52</v>
-      </c>
-      <c r="H31" s="11" t="s">
-        <v>53</v>
       </c>
       <c r="J31" s="11" t="s">
         <v>19</v>
@@ -6815,7 +6826,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
@@ -6839,17 +6850,17 @@
     <row r="2" spans="1:6" ht="26.25" customHeight="1">
       <c r="A2" s="127"/>
       <c r="B2" s="128" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="127"/>
     </row>
     <row r="3" spans="1:6" ht="20" thickBot="1">
       <c r="A3" s="129" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="130"/>
       <c r="C3" s="131" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="20" thickBot="1">
@@ -6869,10 +6880,7 @@
       <c r="B5" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="135">
-        <f>統計數!I6-統計數!O6-統計數!O13</f>
-        <v>0</v>
-      </c>
+      <c r="C5" s="135"/>
       <c r="D5" s="136"/>
       <c r="E5" s="47"/>
       <c r="F5" s="137"/>
@@ -6882,9 +6890,7 @@
       <c r="B6" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="48">
-        <v>0</v>
-      </c>
+      <c r="C6" s="48"/>
       <c r="D6" s="136"/>
     </row>
     <row r="7" spans="1:6" ht="20">
@@ -6892,10 +6898,7 @@
       <c r="B7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="138">
-        <f>統計數!I7-統計數!O7</f>
-        <v>0</v>
-      </c>
+      <c r="C7" s="138"/>
       <c r="D7" s="136"/>
       <c r="E7" s="139"/>
     </row>
@@ -6904,9 +6907,7 @@
       <c r="B8" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="48">
-        <v>0</v>
-      </c>
+      <c r="C8" s="48"/>
       <c r="D8" s="136"/>
     </row>
     <row r="9" spans="1:6" ht="20.5" thickBot="1">
@@ -6933,21 +6934,16 @@
     <row r="11" spans="1:6" ht="17">
       <c r="A11" s="235"/>
       <c r="B11" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="43" t="s">
-        <v>20</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C11" s="43"/>
     </row>
     <row r="12" spans="1:6" ht="20">
       <c r="A12" s="235"/>
       <c r="B12" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="45">
-        <f>統計數!I5-統計數!O5</f>
-        <v>0</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C12" s="45"/>
     </row>
     <row r="13" spans="1:6" ht="20.5" thickBot="1">
       <c r="A13" s="235"/>
@@ -6976,7 +6972,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" s="31"/>
       <c r="E15" s="47"/>
@@ -6984,7 +6980,7 @@
     <row r="16" spans="1:6" ht="20.5" thickBot="1">
       <c r="A16" s="238"/>
       <c r="B16" s="145" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" s="146"/>
       <c r="E16" s="147"/>
@@ -6994,19 +6990,14 @@
       <c r="B17" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="148">
-        <f>統計數!I9-統計數!O9</f>
-        <v>0</v>
-      </c>
+      <c r="C17" s="148"/>
     </row>
     <row r="18" spans="1:6" ht="17">
       <c r="A18" s="238"/>
       <c r="B18" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="37" t="s">
-        <v>21</v>
-      </c>
+      <c r="C18" s="37"/>
     </row>
     <row r="19" spans="1:6" ht="17">
       <c r="A19" s="238"/>
@@ -7045,19 +7036,16 @@
     <row r="23" spans="1:6" ht="17">
       <c r="A23" s="238"/>
       <c r="B23" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="39"/>
     </row>
     <row r="24" spans="1:6" ht="20">
       <c r="A24" s="238"/>
       <c r="B24" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="46">
-        <f>統計數!I8-統計數!O8</f>
-        <v>0</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C24" s="46"/>
     </row>
     <row r="25" spans="1:6" ht="20.5" thickBot="1">
       <c r="A25" s="149"/>
@@ -7072,7 +7060,7 @@
     <row r="26" spans="1:6" ht="30" customHeight="1" thickBot="1">
       <c r="A26" s="150"/>
       <c r="B26" s="132" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="144">
         <f>C21+C25</f>
@@ -7083,7 +7071,7 @@
     </row>
     <row r="27" spans="1:6" ht="42" customHeight="1" thickBot="1">
       <c r="A27" s="232" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B27" s="233"/>
       <c r="C27" s="151">
@@ -7091,7 +7079,7 @@
         <v>0</v>
       </c>
       <c r="D27" s="152" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27" s="153"/>
       <c r="F27" s="154">
@@ -7100,36 +7088,36 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="155" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="156"/>
       <c r="D28" s="157" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E28" s="158"/>
     </row>
     <row r="29" spans="1:6" ht="57.75" customHeight="1">
       <c r="B29" s="5"/>
       <c r="C29" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="159" customFormat="1" ht="18">
       <c r="A30" s="231" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" s="231"/>
       <c r="C30" s="231"/>
     </row>
     <row r="31" spans="1:6">
       <c r="C31" s="126" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="C32" s="126" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="3:4">
@@ -7138,12 +7126,12 @@
     </row>
     <row r="34" spans="3:4">
       <c r="C34" s="126" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="3:4">
       <c r="C37" s="126" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="3:4">
@@ -7153,12 +7141,12 @@
     </row>
     <row r="40" spans="3:4">
       <c r="C40" s="126" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="3:4">
       <c r="C41" s="126" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -7184,14 +7172,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:P27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
   <cols>
     <col min="1" max="2" width="17.75" style="164" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="13.08203125" style="164" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="164" customWidth="1"/>
+    <col min="5" max="7" width="13.08203125" style="164" customWidth="1"/>
     <col min="8" max="8" width="17.5" style="164" customWidth="1"/>
     <col min="9" max="9" width="22.6640625" style="164" customWidth="1"/>
     <col min="10" max="10" width="17.75" style="164" bestFit="1" customWidth="1"/>
@@ -7206,7 +7195,7 @@
       <c r="B3" s="54"/>
       <c r="C3" s="54"/>
       <c r="D3" s="54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E3" s="55"/>
       <c r="F3" s="55"/>
@@ -7223,10 +7212,10 @@
     </row>
     <row r="4" spans="1:16" s="169" customFormat="1" ht="34.5" thickTop="1">
       <c r="A4" s="165" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="166" t="s">
         <v>83</v>
-      </c>
-      <c r="B4" s="166" t="s">
-        <v>84</v>
       </c>
       <c r="C4" s="166">
         <v>1</v>
@@ -7244,39 +7233,39 @@
         <v>5</v>
       </c>
       <c r="H4" s="166" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I4" s="167" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="K4" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="L4" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="M4" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="N4" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="O4" s="168" t="s">
+        <v>76</v>
+      </c>
+      <c r="P4" s="50" t="s">
         <v>77</v>
-      </c>
-      <c r="J4" s="51" t="s">
-        <v>87</v>
-      </c>
-      <c r="K4" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="L4" s="52" t="s">
-        <v>89</v>
-      </c>
-      <c r="M4" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="N4" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="O4" s="168" t="s">
-        <v>77</v>
-      </c>
-      <c r="P4" s="50" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="239" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="166" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" s="170">
         <f>C21+C16</f>
@@ -7291,7 +7280,7 @@
       </c>
       <c r="H5" s="56"/>
       <c r="I5" s="170">
-        <f>SUM(C5:H5)+C12</f>
+        <f>SUM(C5:H5)</f>
         <v>0</v>
       </c>
       <c r="J5" s="171">
@@ -7320,7 +7309,7 @@
     <row r="6" spans="1:16">
       <c r="A6" s="240"/>
       <c r="B6" s="166" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" s="170">
         <f>C22-C16-C15</f>
@@ -7344,9 +7333,9 @@
         <f>SUM(C6:H6)</f>
         <v>0</v>
       </c>
-      <c r="J6" s="177">
-        <f>(C6-P6+C12)*0.5%+(P6*1.5%)</f>
-        <v>0</v>
+      <c r="J6" s="177" t="e">
+        <f>(C6-P6+D12)*0.5%+(P6*1.5%)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="K6" s="178">
         <f>(D6+C13)*2%+0.4</f>
@@ -7358,15 +7347,15 @@
       </c>
       <c r="M6" s="178"/>
       <c r="N6" s="179"/>
-      <c r="O6" s="175">
+      <c r="O6" s="175" t="e">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>#VALUE!</v>
       </c>
       <c r="P6" s="180"/>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="166" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="166"/>
       <c r="C7" s="170">
@@ -7410,10 +7399,10 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="239" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" s="166" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" s="170">
         <f>C24</f>
@@ -7457,7 +7446,7 @@
     <row r="9" spans="1:16">
       <c r="A9" s="240"/>
       <c r="B9" s="166" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="170">
         <f>C25+C15</f>
@@ -7496,7 +7485,9 @@
       <c r="P9" s="180"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="166"/>
+      <c r="A10" s="166" t="s">
+        <v>102</v>
+      </c>
       <c r="B10" s="166"/>
       <c r="C10" s="170"/>
       <c r="D10" s="56"/>
@@ -7504,7 +7495,10 @@
       <c r="F10" s="56"/>
       <c r="G10" s="56"/>
       <c r="H10" s="56"/>
-      <c r="I10" s="170"/>
+      <c r="I10" s="170">
+        <f>SUM(C10:H10)</f>
+        <v>0</v>
+      </c>
       <c r="J10" s="187"/>
       <c r="K10" s="183"/>
       <c r="L10" s="183"/>
@@ -7515,7 +7509,7 @@
     </row>
     <row r="11" spans="1:16" ht="17.5" thickBot="1">
       <c r="A11" s="189" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" s="189"/>
       <c r="C11" s="170">
@@ -7543,12 +7537,12 @@
         <v>0</v>
       </c>
       <c r="I11" s="170">
+        <f>SUM(I5:I10)</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="190" t="e">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="190">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K11" s="191">
         <f t="shared" ref="K11:N11" si="4">SUM(K5:K10)</f>
@@ -7566,9 +7560,9 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O11" s="193">
+      <c r="O11" s="193" t="e">
         <f>SUM(O5:O10)</f>
-        <v>0.4</v>
+        <v>#VALUE!</v>
       </c>
       <c r="P11" s="194">
         <f>SUM(P5:P10)</f>
@@ -7577,42 +7571,46 @@
     </row>
     <row r="12" spans="1:16" ht="17.5" thickTop="1">
       <c r="A12" s="164" t="s">
-        <v>92</v>
+        <v>103</v>
+      </c>
+      <c r="D12" s="164" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="164" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H13" s="164" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="N13" s="195" t="s">
-        <v>102</v>
-      </c>
-      <c r="O13" s="196">
+        <v>100</v>
+      </c>
+      <c r="O13" s="196" t="e">
         <f>P13-O11</f>
-        <v>-0.4</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="164" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G14" s="197" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H14" s="195" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I14" s="195"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="164" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" s="170">
-        <f>I14-C14</f>
+        <v>93</v>
+      </c>
+      <c r="B15" s="241"/>
+      <c r="C15" s="241">
+        <f>I14-I14</f>
         <v>0</v>
       </c>
       <c r="I15" s="196">
@@ -7622,17 +7620,27 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="164" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="164" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="196"/>
+      <c r="C17" s="196">
+        <f>H21</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="198" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B19" s="199"/>
       <c r="C19" s="200"/>
       <c r="D19" s="54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E19" s="55"/>
       <c r="F19" s="55"/>
@@ -7641,10 +7649,10 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="201" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" s="202" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C20" s="166">
         <v>1</v>
@@ -7659,18 +7667,18 @@
         <v>5</v>
       </c>
       <c r="G20" s="166" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H20" s="166" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="239" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21" s="166" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" s="189"/>
       <c r="D21" s="56"/>
@@ -7685,7 +7693,7 @@
     <row r="22" spans="1:8">
       <c r="A22" s="240"/>
       <c r="B22" s="166" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C22" s="189"/>
       <c r="D22" s="56"/>
@@ -7699,10 +7707,10 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="166" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23" s="166" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C23" s="189"/>
       <c r="D23" s="56"/>
@@ -7716,10 +7724,10 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="239" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B24" s="166" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C24" s="189"/>
       <c r="D24" s="56"/>
@@ -7734,7 +7742,7 @@
     <row r="25" spans="1:8">
       <c r="A25" s="240"/>
       <c r="B25" s="166" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C25" s="189"/>
       <c r="D25" s="56"/>
@@ -7748,10 +7756,10 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="203" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B26" s="203" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C26" s="189"/>
       <c r="D26" s="56"/>
@@ -7765,7 +7773,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="198" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B27" s="199"/>
       <c r="C27" s="56">

</xml_diff>

<commit_message>
Auto-committed on 2022/05/24 週二 11:45:35.87
</commit_message>
<xml_diff>
--- a/Program/Other/LM042_底稿_RBC表_會計部_共三份.xlsx
+++ b/Program/Other/LM042_底稿_RBC表_會計部_共三份.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="380" windowWidth="12120" windowHeight="8220"/>
+    <workbookView xWindow="480" yWindow="380" windowWidth="12120" windowHeight="8220" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="YYYMMRBC" sheetId="19" r:id="rId1"/>
@@ -1741,7 +1741,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="102">
+  <borders count="101">
     <border>
       <left/>
       <right/>
@@ -2709,15 +2709,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="8"/>
       </right>
@@ -3527,7 +3518,7 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="242">
+  <cellXfs count="240">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3653,13 +3644,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="80" fillId="0" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3960,7 +3951,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3969,64 +3960,61 @@
     <xf numFmtId="177" fontId="80" fillId="0" borderId="40" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="80" fillId="0" borderId="95" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="80" fillId="0" borderId="78" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="9" fillId="0" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="80" fillId="0" borderId="96" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="80" fillId="0" borderId="79" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="9" fillId="0" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="9" fillId="0" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="91" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="80" fillId="0" borderId="82" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="80" fillId="0" borderId="81" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="80" fillId="0" borderId="41" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="96" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="92" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="80" fillId="0" borderId="91" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="80" fillId="0" borderId="93" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="9" fillId="0" borderId="97" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="93" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="80" fillId="0" borderId="92" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="97" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="80" fillId="0" borderId="94" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="98" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="80" fillId="0" borderId="98" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="80" fillId="0" borderId="99" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4035,10 +4023,7 @@
     <xf numFmtId="177" fontId="80" fillId="0" borderId="100" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="80" fillId="0" borderId="101" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="83" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4055,10 +4040,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4070,6 +4055,9 @@
     <xf numFmtId="182" fontId="25" fillId="0" borderId="21" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="177" fontId="80" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4172,11 +4160,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="80" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="188">
@@ -5906,7 +5891,7 @@
   </sheetPr>
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -5930,85 +5915,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="33.5">
-      <c r="A1" s="207" t="s">
+      <c r="A1" s="206" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="207"/>
-      <c r="C1" s="207"/>
-      <c r="D1" s="207"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="207"/>
-      <c r="G1" s="207"/>
-      <c r="H1" s="207"/>
-      <c r="I1" s="207"/>
-      <c r="J1" s="207"/>
+      <c r="B1" s="206"/>
+      <c r="C1" s="206"/>
+      <c r="D1" s="206"/>
+      <c r="E1" s="206"/>
+      <c r="F1" s="206"/>
+      <c r="G1" s="206"/>
+      <c r="H1" s="206"/>
+      <c r="I1" s="206"/>
+      <c r="J1" s="206"/>
       <c r="K1" s="57"/>
       <c r="L1" s="58"/>
     </row>
     <row r="2" spans="1:12" ht="17">
-      <c r="A2" s="221" t="s">
+      <c r="A2" s="220" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="221"/>
-      <c r="C2" s="221"/>
-      <c r="D2" s="221"/>
-      <c r="E2" s="221"/>
-      <c r="F2" s="221"/>
-      <c r="G2" s="221"/>
-      <c r="H2" s="221"/>
-      <c r="I2" s="221"/>
-      <c r="J2" s="221"/>
+      <c r="B2" s="220"/>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
+      <c r="G2" s="220"/>
+      <c r="H2" s="220"/>
+      <c r="I2" s="220"/>
+      <c r="J2" s="220"/>
       <c r="K2" s="59" t="s">
         <v>26</v>
       </c>
       <c r="L2" s="58"/>
     </row>
     <row r="3" spans="1:12" ht="16" thickBot="1">
-      <c r="A3" s="222"/>
-      <c r="B3" s="222"/>
-      <c r="C3" s="222"/>
-      <c r="D3" s="222"/>
-      <c r="E3" s="222"/>
-      <c r="F3" s="222"/>
-      <c r="G3" s="222"/>
-      <c r="H3" s="222"/>
-      <c r="I3" s="222"/>
-      <c r="J3" s="222"/>
+      <c r="A3" s="221"/>
+      <c r="B3" s="221"/>
+      <c r="C3" s="221"/>
+      <c r="D3" s="221"/>
+      <c r="E3" s="221"/>
+      <c r="F3" s="221"/>
+      <c r="G3" s="221"/>
+      <c r="H3" s="221"/>
+      <c r="I3" s="221"/>
+      <c r="J3" s="221"/>
       <c r="K3" s="60" t="s">
         <v>31</v>
       </c>
       <c r="L3" s="58"/>
     </row>
     <row r="4" spans="1:12" ht="20.149999999999999" customHeight="1" thickBot="1">
-      <c r="A4" s="208" t="s">
+      <c r="A4" s="207" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="209"/>
-      <c r="C4" s="212" t="s">
+      <c r="B4" s="208"/>
+      <c r="C4" s="211" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="214" t="s">
+      <c r="D4" s="213" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="214"/>
-      <c r="F4" s="217" t="s">
+      <c r="E4" s="213"/>
+      <c r="F4" s="216" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="218"/>
-      <c r="H4" s="219" t="s">
+      <c r="G4" s="217"/>
+      <c r="H4" s="218" t="s">
         <v>71</v>
       </c>
-      <c r="I4" s="220"/>
-      <c r="J4" s="215" t="s">
+      <c r="I4" s="219"/>
+      <c r="J4" s="214" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="216"/>
+      <c r="K4" s="215"/>
       <c r="L4" s="58"/>
     </row>
     <row r="5" spans="1:12" ht="20.149999999999999" customHeight="1" thickTop="1">
-      <c r="A5" s="210"/>
-      <c r="B5" s="211"/>
-      <c r="C5" s="213"/>
+      <c r="A5" s="209"/>
+      <c r="B5" s="210"/>
+      <c r="C5" s="212"/>
       <c r="D5" s="61" t="s">
         <v>27</v>
       </c>
@@ -6036,7 +6021,7 @@
       <c r="L5" s="58"/>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
-      <c r="A6" s="223" t="s">
+      <c r="A6" s="222" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="68" t="s">
@@ -6054,7 +6039,7 @@
       <c r="L6" s="58"/>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
-      <c r="A7" s="224"/>
+      <c r="A7" s="223"/>
       <c r="B7" s="75" t="s">
         <v>36</v>
       </c>
@@ -6090,7 +6075,7 @@
       <c r="L7" s="58"/>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1">
-      <c r="A8" s="224"/>
+      <c r="A8" s="223"/>
       <c r="B8" s="75" t="s">
         <v>37</v>
       </c>
@@ -6126,7 +6111,7 @@
       <c r="L8" s="58"/>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1">
-      <c r="A9" s="224"/>
+      <c r="A9" s="223"/>
       <c r="B9" s="75" t="s">
         <v>38</v>
       </c>
@@ -6162,7 +6147,7 @@
       <c r="L9" s="58"/>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1">
-      <c r="A10" s="224"/>
+      <c r="A10" s="223"/>
       <c r="B10" s="75" t="s">
         <v>39</v>
       </c>
@@ -6198,7 +6183,7 @@
       <c r="L10" s="58"/>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1">
-      <c r="A11" s="224"/>
+      <c r="A11" s="223"/>
       <c r="B11" s="83" t="s">
         <v>40</v>
       </c>
@@ -6238,7 +6223,7 @@
       <c r="L11" s="58"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
-      <c r="A12" s="224"/>
+      <c r="A12" s="223"/>
       <c r="B12" s="68" t="s">
         <v>41</v>
       </c>
@@ -6254,7 +6239,7 @@
       <c r="L12" s="58"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
-      <c r="A13" s="224"/>
+      <c r="A13" s="223"/>
       <c r="B13" s="92" t="s">
         <v>42</v>
       </c>
@@ -6282,7 +6267,7 @@
       <c r="L13" s="58"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
-      <c r="A14" s="224"/>
+      <c r="A14" s="223"/>
       <c r="B14" s="92" t="s">
         <v>43</v>
       </c>
@@ -6318,7 +6303,7 @@
       <c r="L14" s="58"/>
     </row>
     <row r="15" spans="1:12" ht="28.9" customHeight="1">
-      <c r="A15" s="224"/>
+      <c r="A15" s="223"/>
       <c r="B15" s="83" t="s">
         <v>44</v>
       </c>
@@ -6358,7 +6343,7 @@
       <c r="L15" s="58"/>
     </row>
     <row r="16" spans="1:12" ht="34.5" customHeight="1" thickBot="1">
-      <c r="A16" s="225"/>
+      <c r="A16" s="224"/>
       <c r="B16" s="98" t="s">
         <v>45</v>
       </c>
@@ -6398,7 +6383,7 @@
       <c r="L16" s="102"/>
     </row>
     <row r="17" spans="1:12" ht="33.75" customHeight="1" thickTop="1">
-      <c r="A17" s="226" t="s">
+      <c r="A17" s="225" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="103" t="s">
@@ -6440,7 +6425,7 @@
       <c r="L17" s="107"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
-      <c r="A18" s="227"/>
+      <c r="A18" s="226"/>
       <c r="B18" s="68" t="s">
         <v>35</v>
       </c>
@@ -6456,7 +6441,7 @@
       <c r="L18" s="58"/>
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
-      <c r="A19" s="227"/>
+      <c r="A19" s="226"/>
       <c r="B19" s="92" t="s">
         <v>47</v>
       </c>
@@ -6492,7 +6477,7 @@
       <c r="L19" s="58"/>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1">
-      <c r="A20" s="227"/>
+      <c r="A20" s="226"/>
       <c r="B20" s="83" t="s">
         <v>48</v>
       </c>
@@ -6532,7 +6517,7 @@
       <c r="L20" s="58"/>
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
-      <c r="A21" s="227"/>
+      <c r="A21" s="226"/>
       <c r="B21" s="68" t="s">
         <v>41</v>
       </c>
@@ -6548,7 +6533,7 @@
       <c r="L21" s="58"/>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
-      <c r="A22" s="227"/>
+      <c r="A22" s="226"/>
       <c r="B22" s="92" t="s">
         <v>42</v>
       </c>
@@ -6582,17 +6567,17 @@
       <c r="L22" s="58"/>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
-      <c r="A23" s="227"/>
+      <c r="A23" s="226"/>
       <c r="B23" s="92" t="s">
         <v>43</v>
       </c>
       <c r="C23" s="76">
         <v>0.23710000000000001</v>
       </c>
-      <c r="D23" s="204">
+      <c r="D23" s="202">
         <v>2232651.96</v>
       </c>
-      <c r="E23" s="204">
+      <c r="E23" s="202">
         <v>2232651.96</v>
       </c>
       <c r="F23" s="27">
@@ -6623,27 +6608,27 @@
         <v>49</v>
       </c>
       <c r="C24" s="99"/>
-      <c r="D24" s="205">
+      <c r="D24" s="203">
         <f>SUM(D22:D23)</f>
         <v>2232651.96</v>
       </c>
-      <c r="E24" s="205">
+      <c r="E24" s="203">
         <f t="shared" ref="E24:I24" si="7">SUM(E22:E23)</f>
         <v>2232651.96</v>
       </c>
-      <c r="F24" s="205">
+      <c r="F24" s="203">
         <f t="shared" si="7"/>
         <v>1293966.6299999999</v>
       </c>
-      <c r="G24" s="205">
+      <c r="G24" s="203">
         <f t="shared" si="7"/>
         <v>306799.48797299998</v>
       </c>
-      <c r="H24" s="205">
+      <c r="H24" s="203">
         <f t="shared" si="7"/>
         <v>1264998.24</v>
       </c>
-      <c r="I24" s="205">
+      <c r="I24" s="203">
         <f t="shared" si="7"/>
         <v>299931.082704</v>
       </c>
@@ -6658,8 +6643,8 @@
       <c r="L24" s="58"/>
     </row>
     <row r="25" spans="1:12" ht="35.15" customHeight="1" thickBot="1">
-      <c r="A25" s="228"/>
-      <c r="B25" s="229"/>
+      <c r="A25" s="227"/>
+      <c r="B25" s="228"/>
       <c r="C25" s="115"/>
       <c r="D25" s="116">
         <f>D16+D17</f>
@@ -6705,8 +6690,8 @@
       <c r="E26" s="119"/>
       <c r="F26" s="119"/>
       <c r="G26" s="119"/>
-      <c r="H26" s="206"/>
-      <c r="I26" s="206"/>
+      <c r="H26" s="205"/>
+      <c r="I26" s="205"/>
       <c r="J26" s="120"/>
       <c r="K26" s="119"/>
       <c r="L26" s="58"/>
@@ -6841,11 +6826,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27.5">
-      <c r="A1" s="230" t="s">
+      <c r="A1" s="229" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="230"/>
-      <c r="C1" s="230"/>
+      <c r="B1" s="229"/>
+      <c r="C1" s="229"/>
     </row>
     <row r="2" spans="1:6" ht="26.25" customHeight="1">
       <c r="A2" s="127"/>
@@ -6864,7 +6849,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="20" thickBot="1">
-      <c r="A4" s="234" t="s">
+      <c r="A4" s="233" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="132" t="s">
@@ -6876,7 +6861,7 @@
       <c r="D4" s="134"/>
     </row>
     <row r="5" spans="1:6" ht="20">
-      <c r="A5" s="235"/>
+      <c r="A5" s="234"/>
       <c r="B5" s="40" t="s">
         <v>8</v>
       </c>
@@ -6886,7 +6871,7 @@
       <c r="F5" s="137"/>
     </row>
     <row r="6" spans="1:6" ht="20">
-      <c r="A6" s="235"/>
+      <c r="A6" s="234"/>
       <c r="B6" s="41" t="s">
         <v>9</v>
       </c>
@@ -6894,7 +6879,7 @@
       <c r="D6" s="136"/>
     </row>
     <row r="7" spans="1:6" ht="20">
-      <c r="A7" s="235"/>
+      <c r="A7" s="234"/>
       <c r="B7" s="41" t="s">
         <v>10</v>
       </c>
@@ -6903,7 +6888,7 @@
       <c r="E7" s="139"/>
     </row>
     <row r="8" spans="1:6" ht="20">
-      <c r="A8" s="235"/>
+      <c r="A8" s="234"/>
       <c r="B8" s="41" t="s">
         <v>11</v>
       </c>
@@ -6911,7 +6896,7 @@
       <c r="D8" s="136"/>
     </row>
     <row r="9" spans="1:6" ht="20.5" thickBot="1">
-      <c r="A9" s="235"/>
+      <c r="A9" s="234"/>
       <c r="B9" s="34" t="s">
         <v>12</v>
       </c>
@@ -6923,7 +6908,7 @@
       <c r="E9" s="140"/>
     </row>
     <row r="10" spans="1:6" ht="17.5" thickBot="1">
-      <c r="A10" s="235"/>
+      <c r="A10" s="234"/>
       <c r="B10" s="141" t="s">
         <v>3</v>
       </c>
@@ -6932,21 +6917,21 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="17">
-      <c r="A11" s="235"/>
+      <c r="A11" s="234"/>
       <c r="B11" s="42" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="43"/>
     </row>
     <row r="12" spans="1:6" ht="20">
-      <c r="A12" s="235"/>
+      <c r="A12" s="234"/>
       <c r="B12" s="44" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="45"/>
     </row>
     <row r="13" spans="1:6" ht="20.5" thickBot="1">
-      <c r="A13" s="235"/>
+      <c r="A13" s="234"/>
       <c r="B13" s="34" t="s">
         <v>13</v>
       </c>
@@ -6956,7 +6941,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" customHeight="1" thickBot="1">
-      <c r="A14" s="236"/>
+      <c r="A14" s="235"/>
       <c r="B14" s="132" t="s">
         <v>14</v>
       </c>
@@ -6968,7 +6953,7 @@
       <c r="F14" s="140"/>
     </row>
     <row r="15" spans="1:6" ht="20.5" thickBot="1">
-      <c r="A15" s="237" t="s">
+      <c r="A15" s="236" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="32" t="s">
@@ -6978,7 +6963,7 @@
       <c r="E15" s="47"/>
     </row>
     <row r="16" spans="1:6" ht="20.5" thickBot="1">
-      <c r="A16" s="238"/>
+      <c r="A16" s="237"/>
       <c r="B16" s="145" t="s">
         <v>62</v>
       </c>
@@ -6986,35 +6971,35 @@
       <c r="E16" s="147"/>
     </row>
     <row r="17" spans="1:6" ht="20">
-      <c r="A17" s="238"/>
+      <c r="A17" s="237"/>
       <c r="B17" s="33" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="148"/>
     </row>
     <row r="18" spans="1:6" ht="17">
-      <c r="A18" s="238"/>
+      <c r="A18" s="237"/>
       <c r="B18" s="36" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="37"/>
     </row>
     <row r="19" spans="1:6" ht="17">
-      <c r="A19" s="238"/>
+      <c r="A19" s="237"/>
       <c r="B19" s="36" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="37"/>
     </row>
     <row r="20" spans="1:6" ht="17">
-      <c r="A20" s="238"/>
+      <c r="A20" s="237"/>
       <c r="B20" s="36" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="37"/>
     </row>
     <row r="21" spans="1:6" ht="20.5" thickBot="1">
-      <c r="A21" s="238"/>
+      <c r="A21" s="237"/>
       <c r="B21" s="34" t="s">
         <v>4</v>
       </c>
@@ -7026,7 +7011,7 @@
       <c r="E21" s="140"/>
     </row>
     <row r="22" spans="1:6" ht="20.5" thickBot="1">
-      <c r="A22" s="238"/>
+      <c r="A22" s="237"/>
       <c r="B22" s="145" t="s">
         <v>3</v>
       </c>
@@ -7034,14 +7019,14 @@
       <c r="E22" s="47"/>
     </row>
     <row r="23" spans="1:6" ht="17">
-      <c r="A23" s="238"/>
+      <c r="A23" s="237"/>
       <c r="B23" s="38" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="39"/>
     </row>
     <row r="24" spans="1:6" ht="20">
-      <c r="A24" s="238"/>
+      <c r="A24" s="237"/>
       <c r="B24" s="44" t="s">
         <v>24</v>
       </c>
@@ -7070,10 +7055,10 @@
       <c r="F26" s="140"/>
     </row>
     <row r="27" spans="1:6" ht="42" customHeight="1" thickBot="1">
-      <c r="A27" s="232" t="s">
+      <c r="A27" s="231" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="233"/>
+      <c r="B27" s="232"/>
       <c r="C27" s="151">
         <f>C14+C26</f>
         <v>0</v>
@@ -7104,11 +7089,11 @@
       </c>
     </row>
     <row r="30" spans="1:6" s="159" customFormat="1" ht="18">
-      <c r="A30" s="231" t="s">
+      <c r="A30" s="230" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="231"/>
-      <c r="C30" s="231"/>
+      <c r="B30" s="230"/>
+      <c r="C30" s="230"/>
     </row>
     <row r="31" spans="1:6">
       <c r="C31" s="126" t="s">
@@ -7172,8 +7157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:P27"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
@@ -7261,7 +7246,7 @@
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="239" t="s">
+      <c r="A5" s="238" t="s">
         <v>78</v>
       </c>
       <c r="B5" s="166" t="s">
@@ -7280,7 +7265,7 @@
       </c>
       <c r="H5" s="56"/>
       <c r="I5" s="170">
-        <f>SUM(C5:H5)</f>
+        <f t="shared" ref="I5:I10" si="0">SUM(C5:H5)</f>
         <v>0</v>
       </c>
       <c r="J5" s="171">
@@ -7295,19 +7280,22 @@
         <f>E5*10%</f>
         <v>0</v>
       </c>
-      <c r="M5" s="173"/>
-      <c r="N5" s="174">
+      <c r="M5" s="172">
+        <f>F5*50%</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="173">
         <f>G5*100%</f>
         <v>0</v>
       </c>
-      <c r="O5" s="175">
-        <f t="shared" ref="O5:O9" si="0">SUM(J5:N5)</f>
-        <v>0</v>
-      </c>
-      <c r="P5" s="176"/>
+      <c r="O5" s="174">
+        <f t="shared" ref="O5:O9" si="1">SUM(J5:N5)</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="175"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="240"/>
+      <c r="A6" s="239"/>
       <c r="B6" s="166" t="s">
         <v>85</v>
       </c>
@@ -7325,33 +7313,39 @@
       </c>
       <c r="F6" s="56"/>
       <c r="G6" s="56">
-        <f t="shared" ref="G6:G9" si="1">F22</f>
+        <f t="shared" ref="G6:G9" si="2">F22</f>
         <v>0</v>
       </c>
       <c r="H6" s="56"/>
       <c r="I6" s="170">
-        <f>SUM(C6:H6)</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="177" t="e">
-        <f>(C6-P6+D12)*0.5%+(P6*1.5%)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K6" s="178">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="176">
+        <f>(C6-P6)*0.5%+(P6*1.5%)</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="177">
         <f>(D6+C13)*2%+0.4</f>
         <v>0.4</v>
       </c>
-      <c r="L6" s="178">
-        <f t="shared" ref="L6:L9" si="2">E6*10%</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="178"/>
-      <c r="N6" s="179"/>
-      <c r="O6" s="175" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P6" s="180"/>
+      <c r="L6" s="177">
+        <f t="shared" ref="L6:M9" si="3">E6*10%</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="177">
+        <f>F6*50%</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="177">
+        <f>G6*100%</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="174">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="P6" s="179"/>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="166" t="s">
@@ -7366,39 +7360,42 @@
       <c r="E7" s="56"/>
       <c r="F7" s="56"/>
       <c r="G7" s="56">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="56"/>
+      <c r="I7" s="180">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="181">
+        <f>(C7-P7)*0.5%+(P7*1.5%)</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="182">
+        <f>D7*2%</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="182">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M7" s="182">
+        <f>F7*50%</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="183">
+        <f>G7*100%</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="174">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H7" s="56"/>
-      <c r="I7" s="181">
-        <f>SUM(C7:H7)</f>
-        <v>0</v>
-      </c>
-      <c r="J7" s="182">
-        <f>(C7-P7)*0.5%+(P7*1.5%)</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="183">
-        <f>D7*2%</f>
-        <v>0</v>
-      </c>
-      <c r="L7" s="183">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M7" s="183"/>
-      <c r="N7" s="184">
-        <f>G7*100%</f>
-        <v>0</v>
-      </c>
-      <c r="O7" s="175">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="185"/>
+      <c r="P7" s="184"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="239" t="s">
+      <c r="A8" s="238" t="s">
         <v>80</v>
       </c>
       <c r="B8" s="166" t="s">
@@ -7412,12 +7409,12 @@
       <c r="E8" s="56"/>
       <c r="F8" s="56"/>
       <c r="G8" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H8" s="56"/>
       <c r="I8" s="170">
-        <f>SUM(C8:H8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J8" s="171">
@@ -7429,22 +7426,25 @@
         <v>0</v>
       </c>
       <c r="L8" s="172">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M8" s="172"/>
-      <c r="N8" s="186">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="172">
+        <f>F8*50%</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="185">
         <f>G8*100%</f>
         <v>0</v>
       </c>
-      <c r="O8" s="175">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P8" s="185"/>
+      <c r="O8" s="174">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="184"/>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="240"/>
+      <c r="A9" s="239"/>
       <c r="B9" s="166" t="s">
         <v>85</v>
       </c>
@@ -7459,30 +7459,39 @@
       <c r="E9" s="56"/>
       <c r="F9" s="56"/>
       <c r="G9" s="56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H9" s="56"/>
       <c r="I9" s="170">
-        <f>SUM(C9:H9)</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="177">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="176">
         <f>(C9-P9)*0.5%+(P9*1.5%)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="178"/>
-      <c r="L9" s="178">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M9" s="178"/>
-      <c r="N9" s="179"/>
-      <c r="O9" s="175">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="180"/>
+      <c r="K9" s="172">
+        <f>D9*2%</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="177">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="177">
+        <f>F9*50%</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="178">
+        <f>G9*100%</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="174">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="179"/>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="166" t="s">
@@ -7496,75 +7505,84 @@
       <c r="G10" s="56"/>
       <c r="H10" s="56"/>
       <c r="I10" s="170">
-        <f>SUM(C10:H10)</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="187"/>
-      <c r="K10" s="183"/>
-      <c r="L10" s="183"/>
-      <c r="M10" s="183"/>
-      <c r="N10" s="184"/>
-      <c r="O10" s="188"/>
-      <c r="P10" s="180"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="176">
+        <f>(C10-P10)*0.5%+(P10*1.5%)</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="182">
+        <f>D10*2%</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="182"/>
+      <c r="M10" s="182"/>
+      <c r="N10" s="183">
+        <f>G10*100%</f>
+        <v>0</v>
+      </c>
+      <c r="O10" s="186"/>
+      <c r="P10" s="179"/>
     </row>
     <row r="11" spans="1:16" ht="17.5" thickBot="1">
-      <c r="A11" s="189" t="s">
+      <c r="A11" s="187" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="189"/>
+      <c r="B11" s="187"/>
       <c r="C11" s="170">
-        <f t="shared" ref="C11:J11" si="3">SUM(C5:C10)</f>
+        <f t="shared" ref="C11:J11" si="4">SUM(C5:C10)</f>
         <v>0</v>
       </c>
       <c r="D11" s="170">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E11" s="170">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F11" s="170">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G11" s="170">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H11" s="170">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I11" s="170">
         <f>SUM(I5:I10)</f>
         <v>0</v>
       </c>
-      <c r="J11" s="190" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K11" s="191">
-        <f t="shared" ref="K11:N11" si="4">SUM(K5:K10)</f>
+      <c r="J11" s="188">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="189">
+        <f t="shared" ref="K11:N11" si="5">SUM(K5:K10)</f>
         <v>0.4</v>
       </c>
-      <c r="L11" s="191">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M11" s="191">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="192">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="193" t="e">
+      <c r="L11" s="189">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="189">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="190">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="191">
         <f>SUM(O5:O10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P11" s="194">
+        <v>0.4</v>
+      </c>
+      <c r="P11" s="192">
         <f>SUM(P5:P10)</f>
         <v>0</v>
       </c>
@@ -7584,36 +7602,36 @@
       <c r="H13" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="N13" s="195" t="s">
+      <c r="N13" s="193" t="s">
         <v>100</v>
       </c>
-      <c r="O13" s="196" t="e">
+      <c r="O13" s="194">
         <f>P13-O11</f>
-        <v>#VALUE!</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="164" t="s">
         <v>92</v>
       </c>
-      <c r="G14" s="197" t="s">
+      <c r="G14" s="195" t="s">
         <v>98</v>
       </c>
-      <c r="H14" s="195" t="s">
+      <c r="H14" s="193" t="s">
         <v>99</v>
       </c>
-      <c r="I14" s="195"/>
+      <c r="I14" s="193"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="164" t="s">
         <v>93</v>
       </c>
-      <c r="B15" s="241"/>
-      <c r="C15" s="241">
+      <c r="B15" s="204"/>
+      <c r="C15" s="204">
         <f>I14-I14</f>
         <v>0</v>
       </c>
-      <c r="I15" s="196">
+      <c r="I15" s="194">
         <f>SUM(I8:I9)-I14</f>
         <v>0</v>
       </c>
@@ -7627,18 +7645,18 @@
       <c r="A17" s="164" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="196"/>
-      <c r="C17" s="196">
+      <c r="B17" s="194"/>
+      <c r="C17" s="194">
         <f>H21</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="198" t="s">
+      <c r="A19" s="196" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="199"/>
-      <c r="C19" s="200"/>
+      <c r="B19" s="197"/>
+      <c r="C19" s="198"/>
       <c r="D19" s="54" t="s">
         <v>75</v>
       </c>
@@ -7648,10 +7666,10 @@
       <c r="H19" s="162"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="201" t="s">
+      <c r="A20" s="199" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="202" t="s">
+      <c r="B20" s="200" t="s">
         <v>96</v>
       </c>
       <c r="C20" s="166">
@@ -7674,13 +7692,13 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="239" t="s">
+      <c r="A21" s="238" t="s">
         <v>78</v>
       </c>
       <c r="B21" s="166" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="189"/>
+      <c r="C21" s="187"/>
       <c r="D21" s="56"/>
       <c r="E21" s="56"/>
       <c r="F21" s="56"/>
@@ -7691,17 +7709,17 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="240"/>
+      <c r="A22" s="239"/>
       <c r="B22" s="166" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="189"/>
+      <c r="C22" s="187"/>
       <c r="D22" s="56"/>
       <c r="E22" s="56"/>
       <c r="F22" s="56"/>
       <c r="G22" s="56"/>
       <c r="H22" s="56">
-        <f t="shared" ref="H22:H27" si="5">SUM(C22:F22)</f>
+        <f t="shared" ref="H22:H27" si="6">SUM(C22:F22)</f>
         <v>0</v>
       </c>
     </row>
@@ -7712,80 +7730,80 @@
       <c r="B23" s="166" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="189"/>
+      <c r="C23" s="187"/>
       <c r="D23" s="56"/>
       <c r="E23" s="56"/>
       <c r="F23" s="56"/>
       <c r="G23" s="56"/>
       <c r="H23" s="56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="239" t="s">
+      <c r="A24" s="238" t="s">
         <v>80</v>
       </c>
       <c r="B24" s="166" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="189"/>
+      <c r="C24" s="187"/>
       <c r="D24" s="56"/>
       <c r="E24" s="56"/>
       <c r="F24" s="56"/>
       <c r="G24" s="56"/>
       <c r="H24" s="56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="240"/>
+      <c r="A25" s="239"/>
       <c r="B25" s="166" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="189"/>
+      <c r="C25" s="187"/>
       <c r="D25" s="56"/>
       <c r="E25" s="56"/>
       <c r="F25" s="56"/>
       <c r="G25" s="56"/>
       <c r="H25" s="56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="203" t="s">
+      <c r="A26" s="201" t="s">
         <v>81</v>
       </c>
-      <c r="B26" s="203" t="s">
+      <c r="B26" s="201" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="189"/>
+      <c r="C26" s="187"/>
       <c r="D26" s="56"/>
       <c r="E26" s="56"/>
       <c r="F26" s="56"/>
       <c r="G26" s="56"/>
       <c r="H26" s="56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="198" t="s">
+      <c r="A27" s="196" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="199"/>
+      <c r="B27" s="197"/>
       <c r="C27" s="56">
         <f>SUM(C21:C25)</f>
         <v>0</v>
       </c>
       <c r="D27" s="56">
-        <f t="shared" ref="D27:E27" si="6">SUM(D21:D25)</f>
+        <f t="shared" ref="D27:E27" si="7">SUM(D21:D25)</f>
         <v>0</v>
       </c>
       <c r="E27" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F27" s="56">
@@ -7794,7 +7812,7 @@
       </c>
       <c r="G27" s="56"/>
       <c r="H27" s="56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -7810,7 +7828,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="F11 C27:F27" formulaRange="1"/>
-    <ignoredError sqref="J6:K6" formula="1"/>
+    <ignoredError sqref="K6" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Auto-committed on 2023/10/02 週一 11:50:58.11
</commit_message>
<xml_diff>
--- a/Program/Other/LM042_底稿_RBC表_會計部_共三份.xlsx
+++ b/Program/Other/LM042_底稿_RBC表_會計部_共三份.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\SKL\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="380" windowWidth="12120" windowHeight="8220" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="384" windowWidth="12120" windowHeight="8220" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="YYYMMRBC" sheetId="19" r:id="rId1"/>
@@ -1741,7 +1741,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="101">
+  <borders count="95">
     <border>
       <left/>
       <right/>
@@ -2708,30 +2708,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="8"/>
       </left>
@@ -2741,26 +2717,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color indexed="64"/>
       </left>
@@ -2789,19 +2745,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="double">
@@ -2818,68 +2761,6 @@
         <color indexed="64"/>
       </right>
       <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -2894,21 +2775,6 @@
       <right style="double">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
       <top style="double">
         <color indexed="64"/>
       </top>
@@ -2916,9 +2782,29 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="double">
         <color indexed="64"/>
       </right>
@@ -2929,10 +2815,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -2945,24 +2831,45 @@
       <left style="double">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom style="double">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom style="double">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -2973,12 +2880,57 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="double">
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -3518,7 +3470,7 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="240">
+  <cellXfs count="236">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3644,13 +3596,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="80" fillId="0" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="80" fillId="0" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="80" fillId="0" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3951,7 +3900,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3960,70 +3909,19 @@
     <xf numFmtId="177" fontId="80" fillId="0" borderId="40" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="80" fillId="0" borderId="95" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="80" fillId="0" borderId="78" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="80" fillId="0" borderId="81" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="80" fillId="0" borderId="41" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="96" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="92" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="80" fillId="0" borderId="91" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="80" fillId="0" borderId="93" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="97" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="80" fillId="0" borderId="98" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="80" fillId="0" borderId="99" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="80" fillId="0" borderId="100" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="80" fillId="0" borderId="83" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="80" fillId="0" borderId="84" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4040,12 +3938,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4058,6 +3956,45 @@
     <xf numFmtId="177" fontId="80" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="80" fillId="0" borderId="85" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="80" fillId="0" borderId="86" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="80" fillId="0" borderId="93" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="80" fillId="0" borderId="94" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4160,8 +4097,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="80" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="188">
@@ -5898,158 +5838,158 @@
       <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.69921875" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="18"/>
-    <col min="4" max="4" width="17.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.796875" style="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.796875" style="1" customWidth="1"/>
     <col min="9" max="9" width="17" style="1" customWidth="1"/>
-    <col min="10" max="11" width="17.58203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="17.59765625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.796875" style="14" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="33.5">
-      <c r="A1" s="206" t="s">
+    <row r="1" spans="1:12" ht="33">
+      <c r="A1" s="201" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="206"/>
-      <c r="C1" s="206"/>
-      <c r="D1" s="206"/>
-      <c r="E1" s="206"/>
-      <c r="F1" s="206"/>
-      <c r="G1" s="206"/>
-      <c r="H1" s="206"/>
-      <c r="I1" s="206"/>
-      <c r="J1" s="206"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="58"/>
-    </row>
-    <row r="2" spans="1:12" ht="17">
-      <c r="A2" s="220" t="s">
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="57"/>
+    </row>
+    <row r="2" spans="1:12" ht="16.2">
+      <c r="A2" s="215" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="220"/>
-      <c r="C2" s="220"/>
-      <c r="D2" s="220"/>
-      <c r="E2" s="220"/>
-      <c r="F2" s="220"/>
-      <c r="G2" s="220"/>
-      <c r="H2" s="220"/>
-      <c r="I2" s="220"/>
-      <c r="J2" s="220"/>
-      <c r="K2" s="59" t="s">
+      <c r="B2" s="215"/>
+      <c r="C2" s="215"/>
+      <c r="D2" s="215"/>
+      <c r="E2" s="215"/>
+      <c r="F2" s="215"/>
+      <c r="G2" s="215"/>
+      <c r="H2" s="215"/>
+      <c r="I2" s="215"/>
+      <c r="J2" s="215"/>
+      <c r="K2" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="58"/>
-    </row>
-    <row r="3" spans="1:12" ht="16" thickBot="1">
-      <c r="A3" s="221"/>
-      <c r="B3" s="221"/>
-      <c r="C3" s="221"/>
-      <c r="D3" s="221"/>
-      <c r="E3" s="221"/>
-      <c r="F3" s="221"/>
-      <c r="G3" s="221"/>
-      <c r="H3" s="221"/>
-      <c r="I3" s="221"/>
-      <c r="J3" s="221"/>
-      <c r="K3" s="60" t="s">
+      <c r="L2" s="57"/>
+    </row>
+    <row r="3" spans="1:12" ht="16.2" thickBot="1">
+      <c r="A3" s="216"/>
+      <c r="B3" s="216"/>
+      <c r="C3" s="216"/>
+      <c r="D3" s="216"/>
+      <c r="E3" s="216"/>
+      <c r="F3" s="216"/>
+      <c r="G3" s="216"/>
+      <c r="H3" s="216"/>
+      <c r="I3" s="216"/>
+      <c r="J3" s="216"/>
+      <c r="K3" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="58"/>
-    </row>
-    <row r="4" spans="1:12" ht="20.149999999999999" customHeight="1" thickBot="1">
-      <c r="A4" s="207" t="s">
+      <c r="L3" s="57"/>
+    </row>
+    <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="A4" s="202" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="208"/>
-      <c r="C4" s="211" t="s">
+      <c r="B4" s="203"/>
+      <c r="C4" s="206" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="213" t="s">
+      <c r="D4" s="208" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="213"/>
-      <c r="F4" s="216" t="s">
+      <c r="E4" s="208"/>
+      <c r="F4" s="211" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="217"/>
-      <c r="H4" s="218" t="s">
+      <c r="G4" s="212"/>
+      <c r="H4" s="213" t="s">
         <v>71</v>
       </c>
-      <c r="I4" s="219"/>
-      <c r="J4" s="214" t="s">
+      <c r="I4" s="214"/>
+      <c r="J4" s="209" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="215"/>
-      <c r="L4" s="58"/>
-    </row>
-    <row r="5" spans="1:12" ht="20.149999999999999" customHeight="1" thickTop="1">
-      <c r="A5" s="209"/>
-      <c r="B5" s="210"/>
-      <c r="C5" s="212"/>
-      <c r="D5" s="61" t="s">
+      <c r="K4" s="210"/>
+      <c r="L4" s="57"/>
+    </row>
+    <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1" thickTop="1">
+      <c r="A5" s="204"/>
+      <c r="B5" s="205"/>
+      <c r="C5" s="207"/>
+      <c r="D5" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="62" t="s">
+      <c r="E5" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="63" t="s">
+      <c r="F5" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="62" t="s">
+      <c r="G5" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="64" t="s">
+      <c r="H5" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="65" t="s">
+      <c r="I5" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="66" t="s">
+      <c r="J5" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="K5" s="67" t="s">
+      <c r="K5" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="L5" s="58"/>
+      <c r="L5" s="57"/>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
-      <c r="A6" s="222" t="s">
+      <c r="A6" s="217" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="70"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="69"/>
       <c r="E6" s="30"/>
       <c r="F6" s="29"/>
       <c r="G6" s="30"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="58"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="57"/>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
-      <c r="A7" s="223"/>
-      <c r="B7" s="75" t="s">
+      <c r="A7" s="218"/>
+      <c r="B7" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="76">
+      <c r="C7" s="75">
         <v>7.1999999999999998E-3</v>
       </c>
-      <c r="D7" s="77">
+      <c r="D7" s="76">
         <v>51114176143.43</v>
       </c>
-      <c r="E7" s="78">
+      <c r="E7" s="77">
         <v>368022068.232696</v>
       </c>
       <c r="F7" s="19">
@@ -6058,34 +5998,34 @@
       <c r="G7" s="20">
         <v>359762122.46476799</v>
       </c>
-      <c r="H7" s="79">
+      <c r="H7" s="78">
         <v>49961192567.160004</v>
       </c>
-      <c r="I7" s="80">
+      <c r="I7" s="79">
         <v>359720586.48355204</v>
       </c>
-      <c r="J7" s="81">
+      <c r="J7" s="80">
         <f>I7-E7</f>
         <v>-8301481.7491439581</v>
       </c>
-      <c r="K7" s="82">
+      <c r="K7" s="81">
         <f>I7-G7</f>
         <v>-41535.981215953827</v>
       </c>
-      <c r="L7" s="58"/>
+      <c r="L7" s="57"/>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1">
-      <c r="A8" s="223"/>
-      <c r="B8" s="75" t="s">
+      <c r="A8" s="218"/>
+      <c r="B8" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="76">
+      <c r="C8" s="75">
         <v>1.0800000000000001E-2</v>
       </c>
-      <c r="D8" s="77">
+      <c r="D8" s="76">
         <v>0</v>
       </c>
-      <c r="E8" s="78">
+      <c r="E8" s="77">
         <v>0</v>
       </c>
       <c r="F8" s="19">
@@ -6094,34 +6034,34 @@
       <c r="G8" s="20">
         <v>0</v>
       </c>
-      <c r="H8" s="79">
+      <c r="H8" s="78">
         <v>0</v>
       </c>
-      <c r="I8" s="80">
+      <c r="I8" s="79">
         <v>0</v>
       </c>
-      <c r="J8" s="81">
+      <c r="J8" s="80">
         <f t="shared" ref="J8:J25" si="0">I8-E8</f>
         <v>0</v>
       </c>
-      <c r="K8" s="82">
+      <c r="K8" s="81">
         <f t="shared" ref="K8:K10" si="1">I8-G8</f>
         <v>0</v>
       </c>
-      <c r="L8" s="58"/>
+      <c r="L8" s="57"/>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1">
-      <c r="A9" s="223"/>
-      <c r="B9" s="75" t="s">
+      <c r="A9" s="218"/>
+      <c r="B9" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="76">
+      <c r="C9" s="75">
         <v>3.9600000000000003E-2</v>
       </c>
-      <c r="D9" s="77">
+      <c r="D9" s="76">
         <v>8811000</v>
       </c>
-      <c r="E9" s="78">
+      <c r="E9" s="77">
         <v>348915.60000000003</v>
       </c>
       <c r="F9" s="19">
@@ -6130,34 +6070,34 @@
       <c r="G9" s="20">
         <v>348915.60000000003</v>
       </c>
-      <c r="H9" s="79">
+      <c r="H9" s="78">
         <v>8811000</v>
       </c>
-      <c r="I9" s="80">
+      <c r="I9" s="79">
         <v>348915.60000000003</v>
       </c>
-      <c r="J9" s="81">
+      <c r="J9" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K9" s="82">
+      <c r="K9" s="81">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L9" s="58"/>
+      <c r="L9" s="57"/>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1">
-      <c r="A10" s="223"/>
-      <c r="B10" s="75" t="s">
+      <c r="A10" s="218"/>
+      <c r="B10" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="76">
+      <c r="C10" s="75">
         <v>4.7999999999999996E-3</v>
       </c>
-      <c r="D10" s="77">
+      <c r="D10" s="76">
         <v>0</v>
       </c>
-      <c r="E10" s="78">
+      <c r="E10" s="77">
         <v>0</v>
       </c>
       <c r="F10" s="19">
@@ -6166,118 +6106,118 @@
       <c r="G10" s="20">
         <v>0</v>
       </c>
-      <c r="H10" s="79">
+      <c r="H10" s="78">
         <v>0</v>
       </c>
-      <c r="I10" s="80">
+      <c r="I10" s="79">
         <v>0</v>
       </c>
-      <c r="J10" s="81">
+      <c r="J10" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K10" s="82">
+      <c r="K10" s="81">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L10" s="58"/>
+      <c r="L10" s="57"/>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1">
-      <c r="A11" s="223"/>
-      <c r="B11" s="83" t="s">
+      <c r="A11" s="218"/>
+      <c r="B11" s="82" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="84"/>
-      <c r="D11" s="85">
+      <c r="C11" s="83"/>
+      <c r="D11" s="84">
         <f>SUM(D7:D10)</f>
         <v>51122987143.43</v>
       </c>
-      <c r="E11" s="85">
+      <c r="E11" s="84">
         <f t="shared" ref="E11:I11" si="2">SUM(E7:E10)</f>
         <v>368370983.83269602</v>
       </c>
-      <c r="F11" s="85">
+      <c r="F11" s="84">
         <f t="shared" si="2"/>
         <v>49975772453.440002</v>
       </c>
-      <c r="G11" s="85">
+      <c r="G11" s="84">
         <f t="shared" si="2"/>
         <v>360111038.06476802</v>
       </c>
-      <c r="H11" s="85">
+      <c r="H11" s="84">
         <f t="shared" si="2"/>
         <v>49970003567.160004</v>
       </c>
-      <c r="I11" s="85">
+      <c r="I11" s="84">
         <f t="shared" si="2"/>
         <v>360069502.08355206</v>
       </c>
-      <c r="J11" s="81">
+      <c r="J11" s="80">
         <f>SUM(J7:J10)</f>
         <v>-8301481.7491439581</v>
       </c>
-      <c r="K11" s="81">
+      <c r="K11" s="80">
         <f>SUM(K7:K10)</f>
         <v>-41535.981215953827</v>
       </c>
-      <c r="L11" s="58"/>
+      <c r="L11" s="57"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
-      <c r="A12" s="223"/>
-      <c r="B12" s="68" t="s">
+      <c r="A12" s="218"/>
+      <c r="B12" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="84"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="88"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="87"/>
       <c r="F12" s="22"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="89"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="90"/>
-      <c r="K12" s="91"/>
-      <c r="L12" s="58"/>
+      <c r="H12" s="88"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="89"/>
+      <c r="K12" s="90"/>
+      <c r="L12" s="57"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
-      <c r="A13" s="223"/>
-      <c r="B13" s="92" t="s">
+      <c r="A13" s="218"/>
+      <c r="B13" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="84"/>
-      <c r="D13" s="93" t="s">
+      <c r="C13" s="83"/>
+      <c r="D13" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="94"/>
+      <c r="E13" s="93"/>
       <c r="F13" s="23" t="s">
         <v>19</v>
       </c>
       <c r="G13" s="20"/>
-      <c r="H13" s="95" t="s">
+      <c r="H13" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="80"/>
-      <c r="J13" s="81">
+      <c r="I13" s="79"/>
+      <c r="J13" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K13" s="82">
+      <c r="K13" s="81">
         <f>I13-G13</f>
         <v>0</v>
       </c>
-      <c r="L13" s="58"/>
+      <c r="L13" s="57"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
-      <c r="A14" s="223"/>
-      <c r="B14" s="92" t="s">
+      <c r="A14" s="218"/>
+      <c r="B14" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="76">
+      <c r="C14" s="75">
         <v>0.23710000000000001</v>
       </c>
-      <c r="D14" s="96">
+      <c r="D14" s="95">
         <v>1598927065.5599997</v>
       </c>
-      <c r="E14" s="78">
+      <c r="E14" s="77">
         <v>379105607.24427593</v>
       </c>
       <c r="F14" s="24">
@@ -6286,172 +6226,172 @@
       <c r="G14" s="20">
         <v>362773397.68381798</v>
       </c>
-      <c r="H14" s="97">
+      <c r="H14" s="96">
         <v>1481432503.3199999</v>
       </c>
-      <c r="I14" s="80">
+      <c r="I14" s="79">
         <v>351247646.53717202</v>
       </c>
-      <c r="J14" s="81">
+      <c r="J14" s="80">
         <f t="shared" si="0"/>
         <v>-27857960.707103908</v>
       </c>
-      <c r="K14" s="82">
+      <c r="K14" s="81">
         <f>I14-G14</f>
         <v>-11525751.146645963</v>
       </c>
-      <c r="L14" s="58"/>
-    </row>
-    <row r="15" spans="1:12" ht="28.9" customHeight="1">
-      <c r="A15" s="223"/>
-      <c r="B15" s="83" t="s">
+      <c r="L14" s="57"/>
+    </row>
+    <row r="15" spans="1:12" ht="28.95" customHeight="1">
+      <c r="A15" s="218"/>
+      <c r="B15" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="84"/>
-      <c r="D15" s="85">
+      <c r="C15" s="83"/>
+      <c r="D15" s="84">
         <f>SUM(D13:D14)</f>
         <v>1598927065.5599997</v>
       </c>
-      <c r="E15" s="85">
+      <c r="E15" s="84">
         <f t="shared" ref="E15:I15" si="3">SUM(E13:E14)</f>
         <v>379105607.24427593</v>
       </c>
-      <c r="F15" s="85">
+      <c r="F15" s="84">
         <f t="shared" si="3"/>
         <v>1530043853.5799999</v>
       </c>
-      <c r="G15" s="85">
+      <c r="G15" s="84">
         <f t="shared" si="3"/>
         <v>362773397.68381798</v>
       </c>
-      <c r="H15" s="85">
+      <c r="H15" s="84">
         <f t="shared" si="3"/>
         <v>1481432503.3199999</v>
       </c>
-      <c r="I15" s="85">
+      <c r="I15" s="84">
         <f t="shared" si="3"/>
         <v>351247646.53717202</v>
       </c>
-      <c r="J15" s="81">
+      <c r="J15" s="80">
         <f>SUM(J13:J14)</f>
         <v>-27857960.707103908</v>
       </c>
-      <c r="K15" s="81">
+      <c r="K15" s="80">
         <f>SUM(K13:K14)</f>
         <v>-11525751.146645963</v>
       </c>
-      <c r="L15" s="58"/>
+      <c r="L15" s="57"/>
     </row>
     <row r="16" spans="1:12" ht="34.5" customHeight="1" thickBot="1">
-      <c r="A16" s="224"/>
-      <c r="B16" s="98" t="s">
+      <c r="A16" s="219"/>
+      <c r="B16" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="99"/>
-      <c r="D16" s="100">
+      <c r="C16" s="98"/>
+      <c r="D16" s="99">
         <f>D11+D15</f>
         <v>52721914208.989998</v>
       </c>
-      <c r="E16" s="100">
+      <c r="E16" s="99">
         <f t="shared" ref="E16:I16" si="4">E11+E15</f>
         <v>747476591.07697201</v>
       </c>
-      <c r="F16" s="100">
+      <c r="F16" s="99">
         <f t="shared" si="4"/>
         <v>51505816307.020004</v>
       </c>
-      <c r="G16" s="100">
+      <c r="G16" s="99">
         <f t="shared" si="4"/>
         <v>722884435.74858594</v>
       </c>
-      <c r="H16" s="100">
+      <c r="H16" s="99">
         <f t="shared" si="4"/>
         <v>51451436070.480003</v>
       </c>
-      <c r="I16" s="100">
+      <c r="I16" s="99">
         <f t="shared" si="4"/>
         <v>711317148.62072408</v>
       </c>
-      <c r="J16" s="81">
+      <c r="J16" s="80">
         <f>J11+J15</f>
         <v>-36159442.456247866</v>
       </c>
-      <c r="K16" s="101">
+      <c r="K16" s="100">
         <f>K11+K15</f>
         <v>-11567287.127861917</v>
       </c>
-      <c r="L16" s="102"/>
+      <c r="L16" s="101"/>
     </row>
     <row r="17" spans="1:12" ht="33.75" customHeight="1" thickTop="1">
-      <c r="A17" s="225" t="s">
+      <c r="A17" s="220" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="103" t="s">
+      <c r="B17" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="104"/>
-      <c r="D17" s="105">
+      <c r="C17" s="103"/>
+      <c r="D17" s="104">
         <f>D20+D24</f>
         <v>1092655178.01</v>
       </c>
-      <c r="E17" s="105">
+      <c r="E17" s="104">
         <f t="shared" ref="E17:I17" si="5">E20+E24</f>
         <v>10083694.14756</v>
       </c>
-      <c r="F17" s="105">
+      <c r="F17" s="104">
         <f t="shared" si="5"/>
         <v>1010803079.88</v>
       </c>
-      <c r="G17" s="105">
+      <c r="G17" s="104">
         <f t="shared" si="5"/>
         <v>7575265.1033729995</v>
       </c>
-      <c r="H17" s="105">
+      <c r="H17" s="104">
         <f t="shared" si="5"/>
         <v>983084610.41999996</v>
       </c>
-      <c r="I17" s="105">
+      <c r="I17" s="104">
         <f t="shared" si="5"/>
         <v>7369032.2903999994</v>
       </c>
-      <c r="J17" s="106">
+      <c r="J17" s="105">
         <f>J20+J24</f>
         <v>-2714661.8571600001</v>
       </c>
-      <c r="K17" s="106">
+      <c r="K17" s="105">
         <f>K20+K24</f>
         <v>-206232.81297300034</v>
       </c>
-      <c r="L17" s="107"/>
+      <c r="L17" s="106"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
-      <c r="A18" s="226"/>
-      <c r="B18" s="68" t="s">
+      <c r="A18" s="221"/>
+      <c r="B18" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="76"/>
-      <c r="D18" s="85"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="84"/>
       <c r="E18" s="21"/>
       <c r="F18" s="28"/>
       <c r="G18" s="21"/>
-      <c r="H18" s="108"/>
-      <c r="I18" s="86"/>
-      <c r="J18" s="81"/>
-      <c r="K18" s="82"/>
-      <c r="L18" s="58"/>
+      <c r="H18" s="107"/>
+      <c r="I18" s="85"/>
+      <c r="J18" s="80"/>
+      <c r="K18" s="81"/>
+      <c r="L18" s="57"/>
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
-      <c r="A19" s="226"/>
-      <c r="B19" s="92" t="s">
+      <c r="A19" s="221"/>
+      <c r="B19" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="76">
+      <c r="C19" s="75">
         <v>7.1999999999999998E-3</v>
       </c>
-      <c r="D19" s="77">
+      <c r="D19" s="76">
         <v>1090422526.05</v>
       </c>
-      <c r="E19" s="78">
+      <c r="E19" s="77">
         <v>7851042.1875599995</v>
       </c>
       <c r="F19" s="19">
@@ -6460,85 +6400,85 @@
       <c r="G19" s="20">
         <v>7268465.6153999995</v>
       </c>
-      <c r="H19" s="79">
+      <c r="H19" s="78">
         <v>981819612.17999995</v>
       </c>
-      <c r="I19" s="80">
+      <c r="I19" s="79">
         <v>7069101.2076959992</v>
       </c>
-      <c r="J19" s="81">
+      <c r="J19" s="80">
         <f t="shared" si="0"/>
         <v>-781940.97986400034</v>
       </c>
-      <c r="K19" s="82">
+      <c r="K19" s="81">
         <f>I19-G19</f>
         <v>-199364.40770400036</v>
       </c>
-      <c r="L19" s="58"/>
+      <c r="L19" s="57"/>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1">
-      <c r="A20" s="226"/>
-      <c r="B20" s="83" t="s">
+      <c r="A20" s="221"/>
+      <c r="B20" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="76"/>
-      <c r="D20" s="85">
+      <c r="C20" s="75"/>
+      <c r="D20" s="84">
         <f>SUM(D19)</f>
         <v>1090422526.05</v>
       </c>
-      <c r="E20" s="85">
+      <c r="E20" s="84">
         <f t="shared" ref="E20:I20" si="6">SUM(E19)</f>
         <v>7851042.1875599995</v>
       </c>
-      <c r="F20" s="85">
+      <c r="F20" s="84">
         <f t="shared" si="6"/>
         <v>1009509113.25</v>
       </c>
-      <c r="G20" s="85">
+      <c r="G20" s="84">
         <f t="shared" si="6"/>
         <v>7268465.6153999995</v>
       </c>
-      <c r="H20" s="85">
+      <c r="H20" s="84">
         <f t="shared" si="6"/>
         <v>981819612.17999995</v>
       </c>
-      <c r="I20" s="85">
+      <c r="I20" s="84">
         <f t="shared" si="6"/>
         <v>7069101.2076959992</v>
       </c>
-      <c r="J20" s="81">
+      <c r="J20" s="80">
         <f>J19</f>
         <v>-781940.97986400034</v>
       </c>
-      <c r="K20" s="81">
+      <c r="K20" s="80">
         <f>K19</f>
         <v>-199364.40770400036</v>
       </c>
-      <c r="L20" s="58"/>
+      <c r="L20" s="57"/>
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
-      <c r="A21" s="226"/>
-      <c r="B21" s="68" t="s">
+      <c r="A21" s="221"/>
+      <c r="B21" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="76"/>
-      <c r="D21" s="85"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="84"/>
       <c r="E21" s="21"/>
       <c r="F21" s="22"/>
       <c r="G21" s="21"/>
-      <c r="H21" s="89"/>
-      <c r="I21" s="86"/>
-      <c r="J21" s="81"/>
-      <c r="K21" s="82"/>
-      <c r="L21" s="58"/>
+      <c r="H21" s="88"/>
+      <c r="I21" s="85"/>
+      <c r="J21" s="80"/>
+      <c r="K21" s="81"/>
+      <c r="L21" s="57"/>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
-      <c r="A22" s="226"/>
-      <c r="B22" s="92" t="s">
+      <c r="A22" s="221"/>
+      <c r="B22" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="76"/>
-      <c r="D22" s="109">
+      <c r="C22" s="75"/>
+      <c r="D22" s="108">
         <v>0</v>
       </c>
       <c r="E22" s="26">
@@ -6550,34 +6490,34 @@
       <c r="G22" s="26">
         <v>0</v>
       </c>
-      <c r="H22" s="110">
+      <c r="H22" s="109">
         <v>0</v>
       </c>
-      <c r="I22" s="111">
+      <c r="I22" s="110">
         <v>0</v>
       </c>
-      <c r="J22" s="81">
+      <c r="J22" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K22" s="82">
+      <c r="K22" s="81">
         <f>I22-G22</f>
         <v>0</v>
       </c>
-      <c r="L22" s="58"/>
+      <c r="L22" s="57"/>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
-      <c r="A23" s="226"/>
-      <c r="B23" s="92" t="s">
+      <c r="A23" s="221"/>
+      <c r="B23" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="76">
+      <c r="C23" s="75">
         <v>0.23710000000000001</v>
       </c>
-      <c r="D23" s="202">
+      <c r="D23" s="184">
         <v>2232651.96</v>
       </c>
-      <c r="E23" s="202">
+      <c r="E23" s="184">
         <v>2232651.96</v>
       </c>
       <c r="F23" s="27">
@@ -6586,133 +6526,133 @@
       <c r="G23" s="20">
         <v>306799.48797299998</v>
       </c>
-      <c r="H23" s="112">
+      <c r="H23" s="111">
         <v>1264998.24</v>
       </c>
-      <c r="I23" s="80">
+      <c r="I23" s="79">
         <v>299931.082704</v>
       </c>
-      <c r="J23" s="81">
+      <c r="J23" s="80">
         <f t="shared" si="0"/>
         <v>-1932720.877296</v>
       </c>
-      <c r="K23" s="82">
+      <c r="K23" s="81">
         <f>I23-G23</f>
         <v>-6868.4052689999808</v>
       </c>
-      <c r="L23" s="58"/>
+      <c r="L23" s="57"/>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1" thickBot="1">
-      <c r="A24" s="113"/>
-      <c r="B24" s="114" t="s">
+      <c r="A24" s="112"/>
+      <c r="B24" s="113" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="99"/>
-      <c r="D24" s="203">
+      <c r="C24" s="98"/>
+      <c r="D24" s="185">
         <f>SUM(D22:D23)</f>
         <v>2232651.96</v>
       </c>
-      <c r="E24" s="203">
+      <c r="E24" s="185">
         <f t="shared" ref="E24:I24" si="7">SUM(E22:E23)</f>
         <v>2232651.96</v>
       </c>
-      <c r="F24" s="203">
+      <c r="F24" s="185">
         <f t="shared" si="7"/>
         <v>1293966.6299999999</v>
       </c>
-      <c r="G24" s="203">
+      <c r="G24" s="185">
         <f t="shared" si="7"/>
         <v>306799.48797299998</v>
       </c>
-      <c r="H24" s="203">
+      <c r="H24" s="185">
         <f t="shared" si="7"/>
         <v>1264998.24</v>
       </c>
-      <c r="I24" s="203">
+      <c r="I24" s="185">
         <f t="shared" si="7"/>
         <v>299931.082704</v>
       </c>
-      <c r="J24" s="101">
+      <c r="J24" s="100">
         <f>SUM(J22:J23)</f>
         <v>-1932720.877296</v>
       </c>
-      <c r="K24" s="101">
+      <c r="K24" s="100">
         <f>SUM(K22:K23)</f>
         <v>-6868.4052689999808</v>
       </c>
-      <c r="L24" s="58"/>
-    </row>
-    <row r="25" spans="1:12" ht="35.15" customHeight="1" thickBot="1">
-      <c r="A25" s="227"/>
-      <c r="B25" s="228"/>
-      <c r="C25" s="115"/>
-      <c r="D25" s="116">
+      <c r="L24" s="57"/>
+    </row>
+    <row r="25" spans="1:12" ht="35.1" customHeight="1" thickBot="1">
+      <c r="A25" s="222"/>
+      <c r="B25" s="223"/>
+      <c r="C25" s="114"/>
+      <c r="D25" s="115">
         <f>D16+D17</f>
         <v>53814569387</v>
       </c>
-      <c r="E25" s="116">
+      <c r="E25" s="115">
         <f t="shared" ref="E25:I25" si="8">E16+E17</f>
         <v>757560285.22453201</v>
       </c>
-      <c r="F25" s="116">
+      <c r="F25" s="115">
         <f t="shared" si="8"/>
         <v>52516619386.900002</v>
       </c>
-      <c r="G25" s="116">
+      <c r="G25" s="115">
         <f t="shared" si="8"/>
         <v>730459700.85195899</v>
       </c>
-      <c r="H25" s="116">
+      <c r="H25" s="115">
         <f t="shared" si="8"/>
         <v>52434520680.900002</v>
       </c>
-      <c r="I25" s="116">
+      <c r="I25" s="115">
         <f t="shared" si="8"/>
         <v>718686180.91112411</v>
       </c>
-      <c r="J25" s="81">
+      <c r="J25" s="80">
         <f t="shared" si="0"/>
         <v>-38874104.313407898</v>
       </c>
-      <c r="K25" s="82">
+      <c r="K25" s="81">
         <f>I25-G25</f>
         <v>-11773519.94083488</v>
       </c>
-      <c r="L25" s="107"/>
+      <c r="L25" s="106"/>
     </row>
     <row r="26" spans="1:12" s="8" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A26" s="117" t="s">
+      <c r="A26" s="116" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="117"/>
-      <c r="C26" s="118"/>
-      <c r="D26" s="119"/>
-      <c r="E26" s="119"/>
-      <c r="F26" s="119"/>
-      <c r="G26" s="119"/>
-      <c r="H26" s="205"/>
-      <c r="I26" s="205"/>
-      <c r="J26" s="120"/>
-      <c r="K26" s="119"/>
-      <c r="L26" s="58"/>
-    </row>
-    <row r="27" spans="1:12" s="6" customFormat="1" ht="17">
-      <c r="A27" s="121" t="s">
+      <c r="B26" s="116"/>
+      <c r="C26" s="117"/>
+      <c r="D26" s="118"/>
+      <c r="E26" s="118"/>
+      <c r="F26" s="118"/>
+      <c r="G26" s="118"/>
+      <c r="H26" s="200"/>
+      <c r="I26" s="200"/>
+      <c r="J26" s="119"/>
+      <c r="K26" s="118"/>
+      <c r="L26" s="57"/>
+    </row>
+    <row r="27" spans="1:12" s="6" customFormat="1" ht="16.2">
+      <c r="A27" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="122"/>
-      <c r="C27" s="123"/>
-      <c r="D27" s="124"/>
-      <c r="E27" s="124"/>
-      <c r="F27" s="124"/>
-      <c r="G27" s="124"/>
-      <c r="H27" s="125"/>
-      <c r="I27" s="124"/>
-      <c r="J27" s="124"/>
-      <c r="K27" s="124"/>
-      <c r="L27" s="58"/>
-    </row>
-    <row r="28" spans="1:12" s="9" customFormat="1" ht="17">
+      <c r="B27" s="121"/>
+      <c r="C27" s="122"/>
+      <c r="D27" s="123"/>
+      <c r="E27" s="123"/>
+      <c r="F27" s="123"/>
+      <c r="G27" s="123"/>
+      <c r="H27" s="124"/>
+      <c r="I27" s="123"/>
+      <c r="J27" s="123"/>
+      <c r="K27" s="123"/>
+      <c r="L27" s="57"/>
+    </row>
+    <row r="28" spans="1:12" s="9" customFormat="1" ht="16.2">
       <c r="A28" s="13"/>
       <c r="B28" s="7"/>
       <c r="C28" s="16"/>
@@ -6726,7 +6666,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="14"/>
     </row>
-    <row r="29" spans="1:12" s="9" customFormat="1" ht="17">
+    <row r="29" spans="1:12" s="9" customFormat="1" ht="16.2">
       <c r="A29" s="13"/>
       <c r="B29" s="7"/>
       <c r="C29" s="16"/>
@@ -6740,7 +6680,7 @@
       <c r="K29" s="3"/>
       <c r="L29" s="14"/>
     </row>
-    <row r="30" spans="1:12" s="9" customFormat="1" ht="17">
+    <row r="30" spans="1:12" s="9" customFormat="1" ht="16.2">
       <c r="A30" s="4"/>
       <c r="B30" s="7"/>
       <c r="C30" s="16"/>
@@ -6754,7 +6694,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="14"/>
     </row>
-    <row r="31" spans="1:12" s="11" customFormat="1" ht="18">
+    <row r="31" spans="1:12" s="11" customFormat="1" ht="17.399999999999999">
       <c r="A31" s="10" t="s">
         <v>19</v>
       </c>
@@ -6774,7 +6714,7 @@
       </c>
       <c r="L31" s="15"/>
     </row>
-    <row r="33" spans="2:2" ht="17">
+    <row r="33" spans="2:2" ht="16.2">
       <c r="B33" s="4"/>
     </row>
   </sheetData>
@@ -6814,89 +6754,89 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.5"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="19.8"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="155" customWidth="1"/>
-    <col min="2" max="2" width="52" style="126" customWidth="1"/>
-    <col min="3" max="3" width="26.83203125" style="126" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="126" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="126" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5" style="126" customWidth="1"/>
-    <col min="7" max="16384" width="8.6640625" style="126"/>
+    <col min="1" max="1" width="11.296875" style="154" customWidth="1"/>
+    <col min="2" max="2" width="52" style="125" customWidth="1"/>
+    <col min="3" max="3" width="26.796875" style="125" customWidth="1"/>
+    <col min="4" max="4" width="10.296875" style="125" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5" style="125" customWidth="1"/>
+    <col min="7" max="16384" width="8.69921875" style="125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27.5">
-      <c r="A1" s="229" t="s">
+    <row r="1" spans="1:6" ht="28.2">
+      <c r="A1" s="224" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="229"/>
-      <c r="C1" s="229"/>
+      <c r="B1" s="224"/>
+      <c r="C1" s="224"/>
     </row>
     <row r="2" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A2" s="127"/>
-      <c r="B2" s="128" t="s">
+      <c r="A2" s="126"/>
+      <c r="B2" s="127" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="127"/>
-    </row>
-    <row r="3" spans="1:6" ht="20" thickBot="1">
-      <c r="A3" s="129" t="s">
+      <c r="C2" s="126"/>
+    </row>
+    <row r="3" spans="1:6" ht="20.399999999999999" thickBot="1">
+      <c r="A3" s="128" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="130"/>
-      <c r="C3" s="131" t="s">
+      <c r="B3" s="129"/>
+      <c r="C3" s="130" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="20" thickBot="1">
-      <c r="A4" s="233" t="s">
+    <row r="4" spans="1:6" ht="20.399999999999999" thickBot="1">
+      <c r="A4" s="228" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="132" t="s">
+      <c r="B4" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="133" t="s">
+      <c r="C4" s="132" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="134"/>
-    </row>
-    <row r="5" spans="1:6" ht="20">
-      <c r="A5" s="234"/>
+      <c r="D4" s="133"/>
+    </row>
+    <row r="5" spans="1:6" ht="20.399999999999999">
+      <c r="A5" s="229"/>
       <c r="B5" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="135"/>
-      <c r="D5" s="136"/>
+      <c r="C5" s="134"/>
+      <c r="D5" s="135"/>
       <c r="E5" s="47"/>
-      <c r="F5" s="137"/>
-    </row>
-    <row r="6" spans="1:6" ht="20">
-      <c r="A6" s="234"/>
+      <c r="F5" s="136"/>
+    </row>
+    <row r="6" spans="1:6" ht="20.399999999999999">
+      <c r="A6" s="229"/>
       <c r="B6" s="41" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="48"/>
-      <c r="D6" s="136"/>
-    </row>
-    <row r="7" spans="1:6" ht="20">
-      <c r="A7" s="234"/>
+      <c r="D6" s="135"/>
+    </row>
+    <row r="7" spans="1:6" ht="20.399999999999999">
+      <c r="A7" s="229"/>
       <c r="B7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="138"/>
-      <c r="D7" s="136"/>
-      <c r="E7" s="139"/>
-    </row>
-    <row r="8" spans="1:6" ht="20">
-      <c r="A8" s="234"/>
+      <c r="C7" s="137"/>
+      <c r="D7" s="135"/>
+      <c r="E7" s="138"/>
+    </row>
+    <row r="8" spans="1:6" ht="20.399999999999999">
+      <c r="A8" s="229"/>
       <c r="B8" s="41" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="48"/>
-      <c r="D8" s="136"/>
-    </row>
-    <row r="9" spans="1:6" ht="20.5" thickBot="1">
-      <c r="A9" s="234"/>
+      <c r="D8" s="135"/>
+    </row>
+    <row r="9" spans="1:6" ht="21.6" thickBot="1">
+      <c r="A9" s="229"/>
       <c r="B9" s="34" t="s">
         <v>12</v>
       </c>
@@ -6904,56 +6844,56 @@
         <f>SUM(C5:C8)</f>
         <v>0</v>
       </c>
-      <c r="D9" s="136"/>
-      <c r="E9" s="140"/>
-    </row>
-    <row r="10" spans="1:6" ht="17.5" thickBot="1">
-      <c r="A10" s="234"/>
-      <c r="B10" s="141" t="s">
+      <c r="D9" s="135"/>
+      <c r="E9" s="139"/>
+    </row>
+    <row r="10" spans="1:6" ht="16.8" thickBot="1">
+      <c r="A10" s="229"/>
+      <c r="B10" s="140" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="142" t="s">
+      <c r="C10" s="141" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17">
-      <c r="A11" s="234"/>
+    <row r="11" spans="1:6" ht="16.2">
+      <c r="A11" s="229"/>
       <c r="B11" s="42" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="43"/>
     </row>
-    <row r="12" spans="1:6" ht="20">
-      <c r="A12" s="234"/>
+    <row r="12" spans="1:6" ht="20.399999999999999">
+      <c r="A12" s="229"/>
       <c r="B12" s="44" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="45"/>
     </row>
-    <row r="13" spans="1:6" ht="20.5" thickBot="1">
-      <c r="A13" s="234"/>
+    <row r="13" spans="1:6" ht="21.6" thickBot="1">
+      <c r="A13" s="229"/>
       <c r="B13" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="143">
+      <c r="C13" s="142">
         <f>SUM(C11:C12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" customHeight="1" thickBot="1">
-      <c r="A14" s="235"/>
-      <c r="B14" s="132" t="s">
+      <c r="A14" s="230"/>
+      <c r="B14" s="131" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="144">
+      <c r="C14" s="143">
         <f>C9+C13</f>
         <v>0</v>
       </c>
       <c r="E14" s="47"/>
-      <c r="F14" s="140"/>
-    </row>
-    <row r="15" spans="1:6" ht="20.5" thickBot="1">
-      <c r="A15" s="236" t="s">
+      <c r="F14" s="139"/>
+    </row>
+    <row r="15" spans="1:6" ht="21.6" thickBot="1">
+      <c r="A15" s="231" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="32" t="s">
@@ -6962,44 +6902,44 @@
       <c r="C15" s="31"/>
       <c r="E15" s="47"/>
     </row>
-    <row r="16" spans="1:6" ht="20.5" thickBot="1">
-      <c r="A16" s="237"/>
-      <c r="B16" s="145" t="s">
+    <row r="16" spans="1:6" ht="21.6" thickBot="1">
+      <c r="A16" s="232"/>
+      <c r="B16" s="144" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="146"/>
-      <c r="E16" s="147"/>
-    </row>
-    <row r="17" spans="1:6" ht="20">
-      <c r="A17" s="237"/>
+      <c r="C16" s="145"/>
+      <c r="E16" s="146"/>
+    </row>
+    <row r="17" spans="1:6" ht="21">
+      <c r="A17" s="232"/>
       <c r="B17" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="148"/>
-    </row>
-    <row r="18" spans="1:6" ht="17">
-      <c r="A18" s="237"/>
+      <c r="C17" s="147"/>
+    </row>
+    <row r="18" spans="1:6" ht="16.2">
+      <c r="A18" s="232"/>
       <c r="B18" s="36" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="37"/>
     </row>
-    <row r="19" spans="1:6" ht="17">
-      <c r="A19" s="237"/>
+    <row r="19" spans="1:6" ht="16.2">
+      <c r="A19" s="232"/>
       <c r="B19" s="36" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="37"/>
     </row>
-    <row r="20" spans="1:6" ht="17">
-      <c r="A20" s="237"/>
+    <row r="20" spans="1:6" ht="16.2">
+      <c r="A20" s="232"/>
       <c r="B20" s="36" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="37"/>
     </row>
-    <row r="21" spans="1:6" ht="20.5" thickBot="1">
-      <c r="A21" s="237"/>
+    <row r="21" spans="1:6" ht="21.6" thickBot="1">
+      <c r="A21" s="232"/>
       <c r="B21" s="34" t="s">
         <v>4</v>
       </c>
@@ -7007,80 +6947,80 @@
         <f>SUM(C17:C20)</f>
         <v>0</v>
       </c>
-      <c r="D21" s="136"/>
-      <c r="E21" s="140"/>
-    </row>
-    <row r="22" spans="1:6" ht="20.5" thickBot="1">
-      <c r="A22" s="237"/>
-      <c r="B22" s="145" t="s">
+      <c r="D21" s="135"/>
+      <c r="E21" s="139"/>
+    </row>
+    <row r="22" spans="1:6" ht="21.6" thickBot="1">
+      <c r="A22" s="232"/>
+      <c r="B22" s="144" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="146"/>
+      <c r="C22" s="145"/>
       <c r="E22" s="47"/>
     </row>
-    <row r="23" spans="1:6" ht="17">
-      <c r="A23" s="237"/>
+    <row r="23" spans="1:6" ht="16.2">
+      <c r="A23" s="232"/>
       <c r="B23" s="38" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="39"/>
     </row>
-    <row r="24" spans="1:6" ht="20">
-      <c r="A24" s="237"/>
+    <row r="24" spans="1:6" ht="20.399999999999999">
+      <c r="A24" s="232"/>
       <c r="B24" s="44" t="s">
         <v>24</v>
       </c>
       <c r="C24" s="46"/>
     </row>
-    <row r="25" spans="1:6" ht="20.5" thickBot="1">
-      <c r="A25" s="149"/>
+    <row r="25" spans="1:6" ht="21.6" thickBot="1">
+      <c r="A25" s="148"/>
       <c r="B25" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="143">
+      <c r="C25" s="142">
         <f>SUM(C23:C24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" customHeight="1" thickBot="1">
-      <c r="A26" s="150"/>
-      <c r="B26" s="132" t="s">
+      <c r="A26" s="149"/>
+      <c r="B26" s="131" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="144">
+      <c r="C26" s="143">
         <f>C21+C25</f>
         <v>0</v>
       </c>
       <c r="E26" s="47"/>
-      <c r="F26" s="140"/>
+      <c r="F26" s="139"/>
     </row>
     <row r="27" spans="1:6" ht="42" customHeight="1" thickBot="1">
-      <c r="A27" s="231" t="s">
+      <c r="A27" s="226" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="232"/>
-      <c r="C27" s="151">
+      <c r="B27" s="227"/>
+      <c r="C27" s="150">
         <f>C14+C26</f>
         <v>0</v>
       </c>
-      <c r="D27" s="152" t="s">
+      <c r="D27" s="151" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="153"/>
-      <c r="F27" s="154">
+      <c r="E27" s="152"/>
+      <c r="F27" s="153">
         <v>9.999847412109375E-2</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="155" t="s">
+      <c r="A28" s="154" t="s">
         <v>74</v>
       </c>
       <c r="B28" s="5"/>
-      <c r="C28" s="156"/>
-      <c r="D28" s="157" t="s">
+      <c r="C28" s="155"/>
+      <c r="D28" s="156" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="158"/>
+      <c r="E28" s="157"/>
     </row>
     <row r="29" spans="1:6" ht="57.75" customHeight="1">
       <c r="B29" s="5"/>
@@ -7088,49 +7028,49 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="159" customFormat="1" ht="18">
-      <c r="A30" s="230" t="s">
+    <row r="30" spans="1:6" s="158" customFormat="1" ht="17.399999999999999">
+      <c r="A30" s="225" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="230"/>
-      <c r="C30" s="230"/>
+      <c r="B30" s="225"/>
+      <c r="C30" s="225"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="C31" s="126" t="s">
+      <c r="C31" s="125" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="C32" s="126" t="s">
+      <c r="C32" s="125" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="33" spans="3:4">
-      <c r="C33" s="160"/>
-      <c r="D33" s="161"/>
+      <c r="C33" s="159"/>
+      <c r="D33" s="160"/>
     </row>
     <row r="34" spans="3:4">
-      <c r="C34" s="126" t="s">
+      <c r="C34" s="125" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="37" spans="3:4">
-      <c r="C37" s="126" t="s">
+      <c r="C37" s="125" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="39" spans="3:4">
-      <c r="C39" s="126" t="s">
+      <c r="C39" s="125" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="40" spans="3:4">
-      <c r="C40" s="126" t="s">
+      <c r="C40" s="125" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="41" spans="3:4">
-      <c r="C41" s="126" t="s">
+      <c r="C41" s="125" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7158,87 +7098,91 @@
   <dimension ref="A3:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="2" width="17.75" style="164" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="16.33203125" style="164" customWidth="1"/>
-    <col min="5" max="7" width="13.08203125" style="164" customWidth="1"/>
-    <col min="8" max="8" width="17.5" style="164" customWidth="1"/>
-    <col min="9" max="9" width="22.6640625" style="164" customWidth="1"/>
-    <col min="10" max="10" width="17.75" style="164" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="11.25" style="164" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" style="164" customWidth="1"/>
-    <col min="16" max="16" width="17.6640625" style="164" customWidth="1"/>
-    <col min="17" max="16384" width="8.6640625" style="164"/>
+    <col min="1" max="2" width="17.69921875" style="163" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.69921875" style="163" customWidth="1"/>
+    <col min="4" max="4" width="16.296875" style="163" customWidth="1"/>
+    <col min="5" max="7" width="13.09765625" style="163" customWidth="1"/>
+    <col min="8" max="8" width="17.5" style="163" customWidth="1"/>
+    <col min="9" max="9" width="22.69921875" style="163" customWidth="1"/>
+    <col min="10" max="10" width="17.69921875" style="163" customWidth="1"/>
+    <col min="11" max="11" width="14.69921875" style="163" customWidth="1"/>
+    <col min="12" max="12" width="13.59765625" style="163" customWidth="1"/>
+    <col min="13" max="13" width="13.3984375" style="163" customWidth="1"/>
+    <col min="14" max="14" width="15.296875" style="163" customWidth="1"/>
+    <col min="15" max="15" width="18.09765625" style="163" customWidth="1"/>
+    <col min="16" max="16" width="20.5" style="163" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.69921875" style="163"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" ht="17.5" thickBot="1">
-      <c r="A3" s="54"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54" t="s">
+    <row r="3" spans="1:16" ht="16.8" thickBot="1">
+      <c r="A3" s="53"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="162"/>
-      <c r="J3" s="163"/>
-      <c r="K3" s="163"/>
-      <c r="L3" s="163"/>
-      <c r="M3" s="163"/>
-      <c r="N3" s="163"/>
-      <c r="O3" s="163"/>
-      <c r="P3" s="163"/>
-    </row>
-    <row r="4" spans="1:16" s="169" customFormat="1" ht="34.5" thickTop="1">
-      <c r="A4" s="165" t="s">
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="162"/>
+      <c r="K3" s="162"/>
+      <c r="L3" s="162"/>
+      <c r="M3" s="162"/>
+      <c r="N3" s="162"/>
+      <c r="O3" s="162"/>
+      <c r="P3" s="162"/>
+    </row>
+    <row r="4" spans="1:16" s="168" customFormat="1" ht="33" thickTop="1">
+      <c r="A4" s="164" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="166" t="s">
+      <c r="B4" s="165" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="166">
+      <c r="C4" s="165">
         <v>1</v>
       </c>
-      <c r="D4" s="166">
+      <c r="D4" s="165">
         <v>2</v>
       </c>
-      <c r="E4" s="166">
+      <c r="E4" s="165">
         <v>3</v>
       </c>
-      <c r="F4" s="166">
+      <c r="F4" s="165">
         <v>4</v>
       </c>
-      <c r="G4" s="166">
+      <c r="G4" s="165">
         <v>5</v>
       </c>
-      <c r="H4" s="166" t="s">
+      <c r="H4" s="165" t="s">
         <v>101</v>
       </c>
-      <c r="I4" s="167" t="s">
+      <c r="I4" s="166" t="s">
         <v>76</v>
       </c>
-      <c r="J4" s="51" t="s">
+      <c r="J4" s="195" t="s">
         <v>86</v>
       </c>
-      <c r="K4" s="52" t="s">
+      <c r="K4" s="196" t="s">
         <v>87</v>
       </c>
-      <c r="L4" s="52" t="s">
+      <c r="L4" s="51" t="s">
         <v>88</v>
       </c>
       <c r="M4" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="N4" s="53" t="s">
+      <c r="N4" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="O4" s="168" t="s">
+      <c r="O4" s="167" t="s">
         <v>76</v>
       </c>
       <c r="P4" s="50" t="s">
@@ -7246,573 +7190,447 @@
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="238" t="s">
+      <c r="A5" s="233" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="166" t="s">
+      <c r="B5" s="165" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="170">
-        <f>C21+C16</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56">
-        <f>F21</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="56"/>
-      <c r="I5" s="170">
+      <c r="C5" s="169"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="169">
         <f t="shared" ref="I5:I10" si="0">SUM(C5:H5)</f>
         <v>0</v>
       </c>
-      <c r="J5" s="171">
-        <f>(C5-P5)*0.5%+(P5*1.5%)</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="172">
-        <f>D5*2%</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="172">
-        <f>E5*10%</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="172">
-        <f>F5*50%</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="173">
-        <f>G5*100%</f>
-        <v>0</v>
-      </c>
-      <c r="O5" s="174">
+      <c r="J5" s="192"/>
+      <c r="K5" s="189"/>
+      <c r="L5" s="191"/>
+      <c r="M5" s="191"/>
+      <c r="N5" s="191"/>
+      <c r="O5" s="187">
         <f t="shared" ref="O5:O9" si="1">SUM(J5:N5)</f>
         <v>0</v>
       </c>
-      <c r="P5" s="175"/>
+      <c r="P5" s="199"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="239"/>
-      <c r="B6" s="166" t="s">
+      <c r="A6" s="234"/>
+      <c r="B6" s="165" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="170">
-        <f>C22-C16-C15</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="56">
-        <f>D22</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="56">
-        <f>E22</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56">
-        <f t="shared" ref="G6:G9" si="2">F22</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="56"/>
-      <c r="I6" s="170">
+      <c r="C6" s="169"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="169">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J6" s="176">
-        <f>(C6-P6)*0.5%+(P6*1.5%)</f>
+      <c r="J6" s="193"/>
+      <c r="K6" s="197"/>
+      <c r="L6" s="190"/>
+      <c r="M6" s="190"/>
+      <c r="N6" s="190"/>
+      <c r="O6" s="187">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K6" s="177">
-        <f>(D6+C13)*2%+0.4</f>
-        <v>0.4</v>
-      </c>
-      <c r="L6" s="177">
-        <f t="shared" ref="L6:M9" si="3">E6*10%</f>
+      <c r="P6" s="199"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="165" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="165"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="170">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M6" s="177">
-        <f>F6*50%</f>
+      <c r="J7" s="192"/>
+      <c r="K7" s="189"/>
+      <c r="L7" s="191"/>
+      <c r="M7" s="191"/>
+      <c r="N7" s="191"/>
+      <c r="O7" s="187">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N6" s="177">
-        <f>G6*100%</f>
+      <c r="P7" s="199"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="233" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="165" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="169"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="169">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O6" s="174">
+      <c r="J8" s="192"/>
+      <c r="K8" s="189"/>
+      <c r="L8" s="191"/>
+      <c r="M8" s="191"/>
+      <c r="N8" s="191"/>
+      <c r="O8" s="187">
         <f t="shared" si="1"/>
-        <v>0.4</v>
-      </c>
-      <c r="P6" s="179"/>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="166" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="166"/>
-      <c r="C7" s="170">
-        <f>C23</f>
         <v>0</v>
       </c>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56">
+      <c r="P8" s="199"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="234"/>
+      <c r="B9" s="165" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="169"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="169">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="193"/>
+      <c r="K9" s="197"/>
+      <c r="L9" s="190"/>
+      <c r="M9" s="190"/>
+      <c r="N9" s="190"/>
+      <c r="O9" s="187">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="199"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="165" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="165"/>
+      <c r="C10" s="169"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="169">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="193"/>
+      <c r="K10" s="189"/>
+      <c r="L10" s="191"/>
+      <c r="M10" s="191"/>
+      <c r="N10" s="191"/>
+      <c r="O10" s="188"/>
+      <c r="P10" s="199"/>
+    </row>
+    <row r="11" spans="1:16" ht="16.8" thickBot="1">
+      <c r="A11" s="171" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="171"/>
+      <c r="C11" s="169">
+        <f t="shared" ref="C11:J11" si="2">SUM(C5:C10)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="169">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H7" s="56"/>
-      <c r="I7" s="180">
-        <f t="shared" si="0"/>
+      <c r="E11" s="169">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J7" s="181">
-        <f>(C7-P7)*0.5%+(P7*1.5%)</f>
+      <c r="F11" s="169">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K7" s="182">
-        <f>D7*2%</f>
+      <c r="G11" s="169">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L7" s="182">
+      <c r="H11" s="169">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="169">
+        <f>SUM(I5:I10)</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="194">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="198">
+        <f t="shared" ref="K11:N11" si="3">SUM(K5:K10)</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="172">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M7" s="182">
-        <f>F7*50%</f>
-        <v>0</v>
-      </c>
-      <c r="N7" s="183">
-        <f>G7*100%</f>
-        <v>0</v>
-      </c>
-      <c r="O7" s="174">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="184"/>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="238" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="166" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="170">
-        <f>C24</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="56"/>
-      <c r="I8" s="170">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="171">
-        <f>(C8-P8)*0.5%+(P8*1.5%)</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="172">
-        <f>D8*2%</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="172">
+      <c r="M11" s="172">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M8" s="172">
-        <f>F8*50%</f>
-        <v>0</v>
-      </c>
-      <c r="N8" s="185">
-        <f>G8*100%</f>
-        <v>0</v>
-      </c>
-      <c r="O8" s="174">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P8" s="184"/>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="239"/>
-      <c r="B9" s="166" t="s">
-        <v>85</v>
-      </c>
-      <c r="C9" s="170">
-        <f>C25+C15</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="56">
-        <f>D25</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="56"/>
-      <c r="I9" s="170">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="176">
-        <f>(C9-P9)*0.5%+(P9*1.5%)</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="172">
-        <f>D9*2%</f>
-        <v>0</v>
-      </c>
-      <c r="L9" s="177">
+      <c r="N11" s="172">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M9" s="177">
-        <f>F9*50%</f>
+      <c r="O11" s="173">
+        <f>SUM(O5:O10)</f>
         <v>0</v>
       </c>
-      <c r="N9" s="178">
-        <f>G9*100%</f>
+      <c r="P11" s="174">
+        <f>SUM(P5:P10)</f>
         <v>0</v>
       </c>
-      <c r="O9" s="174">
-        <f t="shared" si="1"/>
+    </row>
+    <row r="12" spans="1:16" ht="16.8" thickTop="1">
+      <c r="A12" s="163" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="163" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="163" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" s="163" t="s">
+        <v>97</v>
+      </c>
+      <c r="N13" s="175" t="s">
+        <v>100</v>
+      </c>
+      <c r="O13" s="176">
+        <f>P13-O11</f>
         <v>0</v>
       </c>
-      <c r="P9" s="179"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="166" t="s">
-        <v>102</v>
-      </c>
-      <c r="B10" s="166"/>
-      <c r="C10" s="170"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="170">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="163" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="177" t="s">
+        <v>98</v>
+      </c>
+      <c r="H14" s="175" t="s">
+        <v>99</v>
+      </c>
+      <c r="I14" s="175"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="163" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="186"/>
+      <c r="C15" s="235"/>
+      <c r="I15" s="176">
+        <f>SUM(I8:I9)-I14</f>
         <v>0</v>
       </c>
-      <c r="J10" s="176">
-        <f>(C10-P10)*0.5%+(P10*1.5%)</f>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="163" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="163" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="176"/>
+      <c r="C17" s="176">
+        <f>H21</f>
         <v>0</v>
       </c>
-      <c r="K10" s="182">
-        <f>D10*2%</f>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="178" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="179"/>
+      <c r="C19" s="180"/>
+      <c r="D19" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="161"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="181" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="182" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="165">
+        <v>1</v>
+      </c>
+      <c r="D20" s="165">
+        <v>2</v>
+      </c>
+      <c r="E20" s="165">
+        <v>3</v>
+      </c>
+      <c r="F20" s="165">
+        <v>5</v>
+      </c>
+      <c r="G20" s="165" t="s">
+        <v>101</v>
+      </c>
+      <c r="H20" s="165" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="233" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="165" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="171"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="55">
+        <f>SUM(C21:F21)</f>
         <v>0</v>
       </c>
-      <c r="L10" s="182"/>
-      <c r="M10" s="182"/>
-      <c r="N10" s="183">
-        <f>G10*100%</f>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="234"/>
+      <c r="B22" s="165" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="171"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55">
+        <f t="shared" ref="H22:H27" si="4">SUM(C22:F22)</f>
         <v>0</v>
       </c>
-      <c r="O10" s="186"/>
-      <c r="P10" s="179"/>
-    </row>
-    <row r="11" spans="1:16" ht="17.5" thickBot="1">
-      <c r="A11" s="187" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="187"/>
-      <c r="C11" s="170">
-        <f t="shared" ref="C11:J11" si="4">SUM(C5:C10)</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="170">
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="165" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="165" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="171"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="55">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E11" s="170">
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="233" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="165" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="171"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="55">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F11" s="170">
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="234"/>
+      <c r="B25" s="165" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="171"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G11" s="170">
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="183" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="183" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="171"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="55">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H11" s="170">
-        <f t="shared" si="4"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="178" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="179"/>
+      <c r="C27" s="55">
+        <f>SUM(C21:C25)</f>
         <v>0</v>
       </c>
-      <c r="I11" s="170">
-        <f>SUM(I5:I10)</f>
+      <c r="D27" s="55">
+        <f t="shared" ref="D27:E27" si="5">SUM(D21:D25)</f>
         <v>0</v>
       </c>
-      <c r="J11" s="188">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K11" s="189">
-        <f t="shared" ref="K11:N11" si="5">SUM(K5:K10)</f>
-        <v>0.4</v>
-      </c>
-      <c r="L11" s="189">
+      <c r="E27" s="55">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M11" s="189">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="190">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="191">
-        <f>SUM(O5:O10)</f>
-        <v>0.4</v>
-      </c>
-      <c r="P11" s="192">
-        <f>SUM(P5:P10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="17.5" thickTop="1">
-      <c r="A12" s="164" t="s">
-        <v>103</v>
-      </c>
-      <c r="D12" s="164" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="164" t="s">
-        <v>91</v>
-      </c>
-      <c r="H13" s="164" t="s">
-        <v>97</v>
-      </c>
-      <c r="N13" s="193" t="s">
-        <v>100</v>
-      </c>
-      <c r="O13" s="194">
-        <f>P13-O11</f>
-        <v>-0.4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="164" t="s">
-        <v>92</v>
-      </c>
-      <c r="G14" s="195" t="s">
-        <v>98</v>
-      </c>
-      <c r="H14" s="193" t="s">
-        <v>99</v>
-      </c>
-      <c r="I14" s="193"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="164" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15" s="204"/>
-      <c r="C15" s="204">
-        <f>I14-I14</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="194">
-        <f>SUM(I8:I9)-I14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="164" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="164" t="s">
-        <v>105</v>
-      </c>
-      <c r="B17" s="194"/>
-      <c r="C17" s="194">
-        <f>H21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="196" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19" s="197"/>
-      <c r="C19" s="198"/>
-      <c r="D19" s="54" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="162"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="199" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="200" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="166">
-        <v>1</v>
-      </c>
-      <c r="D20" s="166">
-        <v>2</v>
-      </c>
-      <c r="E20" s="166">
-        <v>3</v>
-      </c>
-      <c r="F20" s="166">
-        <v>5</v>
-      </c>
-      <c r="G20" s="166" t="s">
-        <v>101</v>
-      </c>
-      <c r="H20" s="166" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="238" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="166" t="s">
-        <v>84</v>
-      </c>
-      <c r="C21" s="187"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="56">
-        <f>SUM(C21:F21)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="239"/>
-      <c r="B22" s="166" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="187"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="56">
-        <f t="shared" ref="H22:H27" si="6">SUM(C22:F22)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="166" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="166" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" s="187"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="238" t="s">
-        <v>80</v>
-      </c>
-      <c r="B24" s="166" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" s="187"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="56">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="239"/>
-      <c r="B25" s="166" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="187"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="56">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="201" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26" s="201" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="187"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="56"/>
-      <c r="H26" s="56">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="196" t="s">
-        <v>76</v>
-      </c>
-      <c r="B27" s="197"/>
-      <c r="C27" s="56">
-        <f>SUM(C21:C25)</f>
-        <v>0</v>
-      </c>
-      <c r="D27" s="56">
-        <f t="shared" ref="D27:E27" si="7">SUM(D21:D25)</f>
-        <v>0</v>
-      </c>
-      <c r="E27" s="56">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="56">
+      <c r="F27" s="55">
         <f>SUM(F21:F25)</f>
         <v>0</v>
       </c>
-      <c r="G27" s="56"/>
-      <c r="H27" s="56">
-        <f t="shared" si="6"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="55">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -7828,7 +7646,6 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="F11 C27:F27" formulaRange="1"/>
-    <ignoredError sqref="K6" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Auto-committed on 2023/10/04 週三 16:45:07.78
</commit_message>
<xml_diff>
--- a/Program/Other/LM042_底稿_RBC表_會計部_共三份.xlsx
+++ b/Program/Other/LM042_底稿_RBC表_會計部_共三份.xlsx
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="107">
   <si>
     <t>一、非利害關係人放款</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -977,6 +977,10 @@
   </si>
   <si>
     <t>利關人金額</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>淨額</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
@@ -1741,7 +1745,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="95">
+  <borders count="94">
     <border>
       <left/>
       <right/>
@@ -2746,17 +2750,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -2898,19 +2891,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -2928,6 +2908,21 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -3599,9 +3594,6 @@
     <xf numFmtId="0" fontId="80" fillId="0" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="80" fillId="0" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3900,7 +3892,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3915,10 +3907,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="80" fillId="0" borderId="82" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="80" fillId="0" borderId="83" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="80" fillId="0" borderId="84" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="9" fillId="0" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3956,43 +3948,43 @@
     <xf numFmtId="177" fontId="80" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="80" fillId="0" borderId="84" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="80" fillId="0" borderId="85" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="80" fillId="0" borderId="86" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="9" fillId="0" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="9" fillId="0" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="80" fillId="0" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="80" fillId="0" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="177" fontId="9" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="80" fillId="0" borderId="93" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="80" fillId="0" borderId="94" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="80" fillId="0" borderId="91" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="80" fillId="0" borderId="92" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="80" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4100,8 +4092,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="80" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="188">
@@ -5855,141 +5850,141 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="33">
-      <c r="A1" s="201" t="s">
+      <c r="A1" s="200" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="201"/>
-      <c r="I1" s="201"/>
-      <c r="J1" s="201"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="57"/>
+      <c r="B1" s="200"/>
+      <c r="C1" s="200"/>
+      <c r="D1" s="200"/>
+      <c r="E1" s="200"/>
+      <c r="F1" s="200"/>
+      <c r="G1" s="200"/>
+      <c r="H1" s="200"/>
+      <c r="I1" s="200"/>
+      <c r="J1" s="200"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="56"/>
     </row>
     <row r="2" spans="1:12" ht="16.2">
-      <c r="A2" s="215" t="s">
+      <c r="A2" s="214" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="215"/>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
-      <c r="G2" s="215"/>
-      <c r="H2" s="215"/>
-      <c r="I2" s="215"/>
-      <c r="J2" s="215"/>
-      <c r="K2" s="58" t="s">
+      <c r="B2" s="214"/>
+      <c r="C2" s="214"/>
+      <c r="D2" s="214"/>
+      <c r="E2" s="214"/>
+      <c r="F2" s="214"/>
+      <c r="G2" s="214"/>
+      <c r="H2" s="214"/>
+      <c r="I2" s="214"/>
+      <c r="J2" s="214"/>
+      <c r="K2" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="57"/>
+      <c r="L2" s="56"/>
     </row>
     <row r="3" spans="1:12" ht="16.2" thickBot="1">
-      <c r="A3" s="216"/>
-      <c r="B3" s="216"/>
-      <c r="C3" s="216"/>
-      <c r="D3" s="216"/>
-      <c r="E3" s="216"/>
-      <c r="F3" s="216"/>
-      <c r="G3" s="216"/>
-      <c r="H3" s="216"/>
-      <c r="I3" s="216"/>
-      <c r="J3" s="216"/>
-      <c r="K3" s="59" t="s">
+      <c r="A3" s="215"/>
+      <c r="B3" s="215"/>
+      <c r="C3" s="215"/>
+      <c r="D3" s="215"/>
+      <c r="E3" s="215"/>
+      <c r="F3" s="215"/>
+      <c r="G3" s="215"/>
+      <c r="H3" s="215"/>
+      <c r="I3" s="215"/>
+      <c r="J3" s="215"/>
+      <c r="K3" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="57"/>
+      <c r="L3" s="56"/>
     </row>
     <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A4" s="202" t="s">
+      <c r="A4" s="201" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="203"/>
-      <c r="C4" s="206" t="s">
+      <c r="B4" s="202"/>
+      <c r="C4" s="205" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="208" t="s">
+      <c r="D4" s="207" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="208"/>
-      <c r="F4" s="211" t="s">
+      <c r="E4" s="207"/>
+      <c r="F4" s="210" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="212"/>
-      <c r="H4" s="213" t="s">
+      <c r="G4" s="211"/>
+      <c r="H4" s="212" t="s">
         <v>71</v>
       </c>
-      <c r="I4" s="214"/>
-      <c r="J4" s="209" t="s">
+      <c r="I4" s="213"/>
+      <c r="J4" s="208" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="210"/>
-      <c r="L4" s="57"/>
+      <c r="K4" s="209"/>
+      <c r="L4" s="56"/>
     </row>
     <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1" thickTop="1">
-      <c r="A5" s="204"/>
-      <c r="B5" s="205"/>
-      <c r="C5" s="207"/>
-      <c r="D5" s="60" t="s">
+      <c r="A5" s="203"/>
+      <c r="B5" s="204"/>
+      <c r="C5" s="206"/>
+      <c r="D5" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="61" t="s">
+      <c r="E5" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="62" t="s">
+      <c r="F5" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="61" t="s">
+      <c r="G5" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="63" t="s">
+      <c r="H5" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="64" t="s">
+      <c r="I5" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="65" t="s">
+      <c r="J5" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="K5" s="66" t="s">
+      <c r="K5" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="L5" s="57"/>
+      <c r="L5" s="56"/>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
-      <c r="A6" s="217" t="s">
+      <c r="A6" s="216" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="68"/>
-      <c r="D6" s="69"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="68"/>
       <c r="E6" s="30"/>
       <c r="F6" s="29"/>
       <c r="G6" s="30"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="57"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="56"/>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
-      <c r="A7" s="218"/>
-      <c r="B7" s="74" t="s">
+      <c r="A7" s="217"/>
+      <c r="B7" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="75">
+      <c r="C7" s="74">
         <v>7.1999999999999998E-3</v>
       </c>
-      <c r="D7" s="76">
+      <c r="D7" s="75">
         <v>51114176143.43</v>
       </c>
-      <c r="E7" s="77">
+      <c r="E7" s="76">
         <v>368022068.232696</v>
       </c>
       <c r="F7" s="19">
@@ -5998,34 +5993,34 @@
       <c r="G7" s="20">
         <v>359762122.46476799</v>
       </c>
-      <c r="H7" s="78">
+      <c r="H7" s="77">
         <v>49961192567.160004</v>
       </c>
-      <c r="I7" s="79">
+      <c r="I7" s="78">
         <v>359720586.48355204</v>
       </c>
-      <c r="J7" s="80">
+      <c r="J7" s="79">
         <f>I7-E7</f>
         <v>-8301481.7491439581</v>
       </c>
-      <c r="K7" s="81">
+      <c r="K7" s="80">
         <f>I7-G7</f>
         <v>-41535.981215953827</v>
       </c>
-      <c r="L7" s="57"/>
+      <c r="L7" s="56"/>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1">
-      <c r="A8" s="218"/>
-      <c r="B8" s="74" t="s">
+      <c r="A8" s="217"/>
+      <c r="B8" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="75">
+      <c r="C8" s="74">
         <v>1.0800000000000001E-2</v>
       </c>
-      <c r="D8" s="76">
-        <v>0</v>
-      </c>
-      <c r="E8" s="77">
+      <c r="D8" s="75">
+        <v>0</v>
+      </c>
+      <c r="E8" s="76">
         <v>0</v>
       </c>
       <c r="F8" s="19">
@@ -6034,34 +6029,34 @@
       <c r="G8" s="20">
         <v>0</v>
       </c>
-      <c r="H8" s="78">
-        <v>0</v>
-      </c>
-      <c r="I8" s="79">
-        <v>0</v>
-      </c>
-      <c r="J8" s="80">
+      <c r="H8" s="77">
+        <v>0</v>
+      </c>
+      <c r="I8" s="78">
+        <v>0</v>
+      </c>
+      <c r="J8" s="79">
         <f t="shared" ref="J8:J25" si="0">I8-E8</f>
         <v>0</v>
       </c>
-      <c r="K8" s="81">
+      <c r="K8" s="80">
         <f t="shared" ref="K8:K10" si="1">I8-G8</f>
         <v>0</v>
       </c>
-      <c r="L8" s="57"/>
+      <c r="L8" s="56"/>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1">
-      <c r="A9" s="218"/>
-      <c r="B9" s="74" t="s">
+      <c r="A9" s="217"/>
+      <c r="B9" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="75">
+      <c r="C9" s="74">
         <v>3.9600000000000003E-2</v>
       </c>
-      <c r="D9" s="76">
+      <c r="D9" s="75">
         <v>8811000</v>
       </c>
-      <c r="E9" s="77">
+      <c r="E9" s="76">
         <v>348915.60000000003</v>
       </c>
       <c r="F9" s="19">
@@ -6070,34 +6065,34 @@
       <c r="G9" s="20">
         <v>348915.60000000003</v>
       </c>
-      <c r="H9" s="78">
+      <c r="H9" s="77">
         <v>8811000</v>
       </c>
-      <c r="I9" s="79">
+      <c r="I9" s="78">
         <v>348915.60000000003</v>
       </c>
-      <c r="J9" s="80">
+      <c r="J9" s="79">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K9" s="81">
+      <c r="K9" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L9" s="57"/>
+      <c r="L9" s="56"/>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1">
-      <c r="A10" s="218"/>
-      <c r="B10" s="74" t="s">
+      <c r="A10" s="217"/>
+      <c r="B10" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="75">
+      <c r="C10" s="74">
         <v>4.7999999999999996E-3</v>
       </c>
-      <c r="D10" s="76">
-        <v>0</v>
-      </c>
-      <c r="E10" s="77">
+      <c r="D10" s="75">
+        <v>0</v>
+      </c>
+      <c r="E10" s="76">
         <v>0</v>
       </c>
       <c r="F10" s="19">
@@ -6106,118 +6101,118 @@
       <c r="G10" s="20">
         <v>0</v>
       </c>
-      <c r="H10" s="78">
-        <v>0</v>
-      </c>
-      <c r="I10" s="79">
-        <v>0</v>
-      </c>
-      <c r="J10" s="80">
+      <c r="H10" s="77">
+        <v>0</v>
+      </c>
+      <c r="I10" s="78">
+        <v>0</v>
+      </c>
+      <c r="J10" s="79">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K10" s="81">
+      <c r="K10" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L10" s="57"/>
+      <c r="L10" s="56"/>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1">
-      <c r="A11" s="218"/>
-      <c r="B11" s="82" t="s">
+      <c r="A11" s="217"/>
+      <c r="B11" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="83"/>
-      <c r="D11" s="84">
+      <c r="C11" s="82"/>
+      <c r="D11" s="83">
         <f>SUM(D7:D10)</f>
         <v>51122987143.43</v>
       </c>
-      <c r="E11" s="84">
+      <c r="E11" s="83">
         <f t="shared" ref="E11:I11" si="2">SUM(E7:E10)</f>
         <v>368370983.83269602</v>
       </c>
-      <c r="F11" s="84">
+      <c r="F11" s="83">
         <f t="shared" si="2"/>
         <v>49975772453.440002</v>
       </c>
-      <c r="G11" s="84">
+      <c r="G11" s="83">
         <f t="shared" si="2"/>
         <v>360111038.06476802</v>
       </c>
-      <c r="H11" s="84">
+      <c r="H11" s="83">
         <f t="shared" si="2"/>
         <v>49970003567.160004</v>
       </c>
-      <c r="I11" s="84">
+      <c r="I11" s="83">
         <f t="shared" si="2"/>
         <v>360069502.08355206</v>
       </c>
-      <c r="J11" s="80">
+      <c r="J11" s="79">
         <f>SUM(J7:J10)</f>
         <v>-8301481.7491439581</v>
       </c>
-      <c r="K11" s="80">
+      <c r="K11" s="79">
         <f>SUM(K7:K10)</f>
         <v>-41535.981215953827</v>
       </c>
-      <c r="L11" s="57"/>
+      <c r="L11" s="56"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
-      <c r="A12" s="218"/>
-      <c r="B12" s="67" t="s">
+      <c r="A12" s="217"/>
+      <c r="B12" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="83"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="87"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="86"/>
       <c r="F12" s="22"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="79"/>
-      <c r="J12" s="89"/>
-      <c r="K12" s="90"/>
-      <c r="L12" s="57"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="88"/>
+      <c r="K12" s="89"/>
+      <c r="L12" s="56"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
-      <c r="A13" s="218"/>
-      <c r="B13" s="91" t="s">
+      <c r="A13" s="217"/>
+      <c r="B13" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="83"/>
-      <c r="D13" s="92" t="s">
+      <c r="C13" s="82"/>
+      <c r="D13" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="93"/>
+      <c r="E13" s="92"/>
       <c r="F13" s="23" t="s">
         <v>19</v>
       </c>
       <c r="G13" s="20"/>
-      <c r="H13" s="94" t="s">
+      <c r="H13" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="79"/>
-      <c r="J13" s="80">
+      <c r="I13" s="78"/>
+      <c r="J13" s="79">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K13" s="81">
+      <c r="K13" s="80">
         <f>I13-G13</f>
         <v>0</v>
       </c>
-      <c r="L13" s="57"/>
+      <c r="L13" s="56"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
-      <c r="A14" s="218"/>
-      <c r="B14" s="91" t="s">
+      <c r="A14" s="217"/>
+      <c r="B14" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="75">
+      <c r="C14" s="74">
         <v>0.23710000000000001</v>
       </c>
-      <c r="D14" s="95">
+      <c r="D14" s="94">
         <v>1598927065.5599997</v>
       </c>
-      <c r="E14" s="77">
+      <c r="E14" s="76">
         <v>379105607.24427593</v>
       </c>
       <c r="F14" s="24">
@@ -6226,172 +6221,172 @@
       <c r="G14" s="20">
         <v>362773397.68381798</v>
       </c>
-      <c r="H14" s="96">
+      <c r="H14" s="95">
         <v>1481432503.3199999</v>
       </c>
-      <c r="I14" s="79">
+      <c r="I14" s="78">
         <v>351247646.53717202</v>
       </c>
-      <c r="J14" s="80">
+      <c r="J14" s="79">
         <f t="shared" si="0"/>
         <v>-27857960.707103908</v>
       </c>
-      <c r="K14" s="81">
+      <c r="K14" s="80">
         <f>I14-G14</f>
         <v>-11525751.146645963</v>
       </c>
-      <c r="L14" s="57"/>
+      <c r="L14" s="56"/>
     </row>
     <row r="15" spans="1:12" ht="28.95" customHeight="1">
-      <c r="A15" s="218"/>
-      <c r="B15" s="82" t="s">
+      <c r="A15" s="217"/>
+      <c r="B15" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="83"/>
-      <c r="D15" s="84">
+      <c r="C15" s="82"/>
+      <c r="D15" s="83">
         <f>SUM(D13:D14)</f>
         <v>1598927065.5599997</v>
       </c>
-      <c r="E15" s="84">
+      <c r="E15" s="83">
         <f t="shared" ref="E15:I15" si="3">SUM(E13:E14)</f>
         <v>379105607.24427593</v>
       </c>
-      <c r="F15" s="84">
+      <c r="F15" s="83">
         <f t="shared" si="3"/>
         <v>1530043853.5799999</v>
       </c>
-      <c r="G15" s="84">
+      <c r="G15" s="83">
         <f t="shared" si="3"/>
         <v>362773397.68381798</v>
       </c>
-      <c r="H15" s="84">
+      <c r="H15" s="83">
         <f t="shared" si="3"/>
         <v>1481432503.3199999</v>
       </c>
-      <c r="I15" s="84">
+      <c r="I15" s="83">
         <f t="shared" si="3"/>
         <v>351247646.53717202</v>
       </c>
-      <c r="J15" s="80">
+      <c r="J15" s="79">
         <f>SUM(J13:J14)</f>
         <v>-27857960.707103908</v>
       </c>
-      <c r="K15" s="80">
+      <c r="K15" s="79">
         <f>SUM(K13:K14)</f>
         <v>-11525751.146645963</v>
       </c>
-      <c r="L15" s="57"/>
+      <c r="L15" s="56"/>
     </row>
     <row r="16" spans="1:12" ht="34.5" customHeight="1" thickBot="1">
-      <c r="A16" s="219"/>
-      <c r="B16" s="97" t="s">
+      <c r="A16" s="218"/>
+      <c r="B16" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="98"/>
-      <c r="D16" s="99">
+      <c r="C16" s="97"/>
+      <c r="D16" s="98">
         <f>D11+D15</f>
         <v>52721914208.989998</v>
       </c>
-      <c r="E16" s="99">
+      <c r="E16" s="98">
         <f t="shared" ref="E16:I16" si="4">E11+E15</f>
         <v>747476591.07697201</v>
       </c>
-      <c r="F16" s="99">
+      <c r="F16" s="98">
         <f t="shared" si="4"/>
         <v>51505816307.020004</v>
       </c>
-      <c r="G16" s="99">
+      <c r="G16" s="98">
         <f t="shared" si="4"/>
         <v>722884435.74858594</v>
       </c>
-      <c r="H16" s="99">
+      <c r="H16" s="98">
         <f t="shared" si="4"/>
         <v>51451436070.480003</v>
       </c>
-      <c r="I16" s="99">
+      <c r="I16" s="98">
         <f t="shared" si="4"/>
         <v>711317148.62072408</v>
       </c>
-      <c r="J16" s="80">
+      <c r="J16" s="79">
         <f>J11+J15</f>
         <v>-36159442.456247866</v>
       </c>
-      <c r="K16" s="100">
+      <c r="K16" s="99">
         <f>K11+K15</f>
         <v>-11567287.127861917</v>
       </c>
-      <c r="L16" s="101"/>
+      <c r="L16" s="100"/>
     </row>
     <row r="17" spans="1:12" ht="33.75" customHeight="1" thickTop="1">
-      <c r="A17" s="220" t="s">
+      <c r="A17" s="219" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="102" t="s">
+      <c r="B17" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="103"/>
-      <c r="D17" s="104">
+      <c r="C17" s="102"/>
+      <c r="D17" s="103">
         <f>D20+D24</f>
         <v>1092655178.01</v>
       </c>
-      <c r="E17" s="104">
+      <c r="E17" s="103">
         <f t="shared" ref="E17:I17" si="5">E20+E24</f>
         <v>10083694.14756</v>
       </c>
-      <c r="F17" s="104">
+      <c r="F17" s="103">
         <f t="shared" si="5"/>
         <v>1010803079.88</v>
       </c>
-      <c r="G17" s="104">
+      <c r="G17" s="103">
         <f t="shared" si="5"/>
         <v>7575265.1033729995</v>
       </c>
-      <c r="H17" s="104">
+      <c r="H17" s="103">
         <f t="shared" si="5"/>
         <v>983084610.41999996</v>
       </c>
-      <c r="I17" s="104">
+      <c r="I17" s="103">
         <f t="shared" si="5"/>
         <v>7369032.2903999994</v>
       </c>
-      <c r="J17" s="105">
+      <c r="J17" s="104">
         <f>J20+J24</f>
         <v>-2714661.8571600001</v>
       </c>
-      <c r="K17" s="105">
+      <c r="K17" s="104">
         <f>K20+K24</f>
         <v>-206232.81297300034</v>
       </c>
-      <c r="L17" s="106"/>
+      <c r="L17" s="105"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
-      <c r="A18" s="221"/>
-      <c r="B18" s="67" t="s">
+      <c r="A18" s="220"/>
+      <c r="B18" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="75"/>
-      <c r="D18" s="84"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="83"/>
       <c r="E18" s="21"/>
       <c r="F18" s="28"/>
       <c r="G18" s="21"/>
-      <c r="H18" s="107"/>
-      <c r="I18" s="85"/>
-      <c r="J18" s="80"/>
-      <c r="K18" s="81"/>
-      <c r="L18" s="57"/>
+      <c r="H18" s="106"/>
+      <c r="I18" s="84"/>
+      <c r="J18" s="79"/>
+      <c r="K18" s="80"/>
+      <c r="L18" s="56"/>
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
-      <c r="A19" s="221"/>
-      <c r="B19" s="91" t="s">
+      <c r="A19" s="220"/>
+      <c r="B19" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="75">
+      <c r="C19" s="74">
         <v>7.1999999999999998E-3</v>
       </c>
-      <c r="D19" s="76">
+      <c r="D19" s="75">
         <v>1090422526.05</v>
       </c>
-      <c r="E19" s="77">
+      <c r="E19" s="76">
         <v>7851042.1875599995</v>
       </c>
       <c r="F19" s="19">
@@ -6400,85 +6395,85 @@
       <c r="G19" s="20">
         <v>7268465.6153999995</v>
       </c>
-      <c r="H19" s="78">
+      <c r="H19" s="77">
         <v>981819612.17999995</v>
       </c>
-      <c r="I19" s="79">
+      <c r="I19" s="78">
         <v>7069101.2076959992</v>
       </c>
-      <c r="J19" s="80">
+      <c r="J19" s="79">
         <f t="shared" si="0"/>
         <v>-781940.97986400034</v>
       </c>
-      <c r="K19" s="81">
+      <c r="K19" s="80">
         <f>I19-G19</f>
         <v>-199364.40770400036</v>
       </c>
-      <c r="L19" s="57"/>
+      <c r="L19" s="56"/>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1">
-      <c r="A20" s="221"/>
-      <c r="B20" s="82" t="s">
+      <c r="A20" s="220"/>
+      <c r="B20" s="81" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="75"/>
-      <c r="D20" s="84">
+      <c r="C20" s="74"/>
+      <c r="D20" s="83">
         <f>SUM(D19)</f>
         <v>1090422526.05</v>
       </c>
-      <c r="E20" s="84">
+      <c r="E20" s="83">
         <f t="shared" ref="E20:I20" si="6">SUM(E19)</f>
         <v>7851042.1875599995</v>
       </c>
-      <c r="F20" s="84">
+      <c r="F20" s="83">
         <f t="shared" si="6"/>
         <v>1009509113.25</v>
       </c>
-      <c r="G20" s="84">
+      <c r="G20" s="83">
         <f t="shared" si="6"/>
         <v>7268465.6153999995</v>
       </c>
-      <c r="H20" s="84">
+      <c r="H20" s="83">
         <f t="shared" si="6"/>
         <v>981819612.17999995</v>
       </c>
-      <c r="I20" s="84">
+      <c r="I20" s="83">
         <f t="shared" si="6"/>
         <v>7069101.2076959992</v>
       </c>
-      <c r="J20" s="80">
+      <c r="J20" s="79">
         <f>J19</f>
         <v>-781940.97986400034</v>
       </c>
-      <c r="K20" s="80">
+      <c r="K20" s="79">
         <f>K19</f>
         <v>-199364.40770400036</v>
       </c>
-      <c r="L20" s="57"/>
+      <c r="L20" s="56"/>
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
-      <c r="A21" s="221"/>
-      <c r="B21" s="67" t="s">
+      <c r="A21" s="220"/>
+      <c r="B21" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="75"/>
-      <c r="D21" s="84"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="83"/>
       <c r="E21" s="21"/>
       <c r="F21" s="22"/>
       <c r="G21" s="21"/>
-      <c r="H21" s="88"/>
-      <c r="I21" s="85"/>
-      <c r="J21" s="80"/>
-      <c r="K21" s="81"/>
-      <c r="L21" s="57"/>
+      <c r="H21" s="87"/>
+      <c r="I21" s="84"/>
+      <c r="J21" s="79"/>
+      <c r="K21" s="80"/>
+      <c r="L21" s="56"/>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
-      <c r="A22" s="221"/>
-      <c r="B22" s="91" t="s">
+      <c r="A22" s="220"/>
+      <c r="B22" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="75"/>
-      <c r="D22" s="108">
+      <c r="C22" s="74"/>
+      <c r="D22" s="107">
         <v>0</v>
       </c>
       <c r="E22" s="26">
@@ -6490,34 +6485,34 @@
       <c r="G22" s="26">
         <v>0</v>
       </c>
-      <c r="H22" s="109">
-        <v>0</v>
-      </c>
-      <c r="I22" s="110">
-        <v>0</v>
-      </c>
-      <c r="J22" s="80">
+      <c r="H22" s="108">
+        <v>0</v>
+      </c>
+      <c r="I22" s="109">
+        <v>0</v>
+      </c>
+      <c r="J22" s="79">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K22" s="81">
+      <c r="K22" s="80">
         <f>I22-G22</f>
         <v>0</v>
       </c>
-      <c r="L22" s="57"/>
+      <c r="L22" s="56"/>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
-      <c r="A23" s="221"/>
-      <c r="B23" s="91" t="s">
+      <c r="A23" s="220"/>
+      <c r="B23" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="75">
+      <c r="C23" s="74">
         <v>0.23710000000000001</v>
       </c>
-      <c r="D23" s="184">
+      <c r="D23" s="183">
         <v>2232651.96</v>
       </c>
-      <c r="E23" s="184">
+      <c r="E23" s="183">
         <v>2232651.96</v>
       </c>
       <c r="F23" s="27">
@@ -6526,131 +6521,131 @@
       <c r="G23" s="20">
         <v>306799.48797299998</v>
       </c>
-      <c r="H23" s="111">
+      <c r="H23" s="110">
         <v>1264998.24</v>
       </c>
-      <c r="I23" s="79">
+      <c r="I23" s="78">
         <v>299931.082704</v>
       </c>
-      <c r="J23" s="80">
+      <c r="J23" s="79">
         <f t="shared" si="0"/>
         <v>-1932720.877296</v>
       </c>
-      <c r="K23" s="81">
+      <c r="K23" s="80">
         <f>I23-G23</f>
         <v>-6868.4052689999808</v>
       </c>
-      <c r="L23" s="57"/>
+      <c r="L23" s="56"/>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1" thickBot="1">
-      <c r="A24" s="112"/>
-      <c r="B24" s="113" t="s">
+      <c r="A24" s="111"/>
+      <c r="B24" s="112" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="98"/>
-      <c r="D24" s="185">
+      <c r="C24" s="97"/>
+      <c r="D24" s="184">
         <f>SUM(D22:D23)</f>
         <v>2232651.96</v>
       </c>
-      <c r="E24" s="185">
+      <c r="E24" s="184">
         <f t="shared" ref="E24:I24" si="7">SUM(E22:E23)</f>
         <v>2232651.96</v>
       </c>
-      <c r="F24" s="185">
+      <c r="F24" s="184">
         <f t="shared" si="7"/>
         <v>1293966.6299999999</v>
       </c>
-      <c r="G24" s="185">
+      <c r="G24" s="184">
         <f t="shared" si="7"/>
         <v>306799.48797299998</v>
       </c>
-      <c r="H24" s="185">
+      <c r="H24" s="184">
         <f t="shared" si="7"/>
         <v>1264998.24</v>
       </c>
-      <c r="I24" s="185">
+      <c r="I24" s="184">
         <f t="shared" si="7"/>
         <v>299931.082704</v>
       </c>
-      <c r="J24" s="100">
+      <c r="J24" s="99">
         <f>SUM(J22:J23)</f>
         <v>-1932720.877296</v>
       </c>
-      <c r="K24" s="100">
+      <c r="K24" s="99">
         <f>SUM(K22:K23)</f>
         <v>-6868.4052689999808</v>
       </c>
-      <c r="L24" s="57"/>
+      <c r="L24" s="56"/>
     </row>
     <row r="25" spans="1:12" ht="35.1" customHeight="1" thickBot="1">
-      <c r="A25" s="222"/>
-      <c r="B25" s="223"/>
-      <c r="C25" s="114"/>
-      <c r="D25" s="115">
+      <c r="A25" s="221"/>
+      <c r="B25" s="222"/>
+      <c r="C25" s="113"/>
+      <c r="D25" s="114">
         <f>D16+D17</f>
         <v>53814569387</v>
       </c>
-      <c r="E25" s="115">
+      <c r="E25" s="114">
         <f t="shared" ref="E25:I25" si="8">E16+E17</f>
         <v>757560285.22453201</v>
       </c>
-      <c r="F25" s="115">
+      <c r="F25" s="114">
         <f t="shared" si="8"/>
         <v>52516619386.900002</v>
       </c>
-      <c r="G25" s="115">
+      <c r="G25" s="114">
         <f t="shared" si="8"/>
         <v>730459700.85195899</v>
       </c>
-      <c r="H25" s="115">
+      <c r="H25" s="114">
         <f t="shared" si="8"/>
         <v>52434520680.900002</v>
       </c>
-      <c r="I25" s="115">
+      <c r="I25" s="114">
         <f t="shared" si="8"/>
         <v>718686180.91112411</v>
       </c>
-      <c r="J25" s="80">
+      <c r="J25" s="79">
         <f t="shared" si="0"/>
         <v>-38874104.313407898</v>
       </c>
-      <c r="K25" s="81">
+      <c r="K25" s="80">
         <f>I25-G25</f>
         <v>-11773519.94083488</v>
       </c>
-      <c r="L25" s="106"/>
+      <c r="L25" s="105"/>
     </row>
     <row r="26" spans="1:12" s="8" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A26" s="116" t="s">
+      <c r="A26" s="115" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="116"/>
-      <c r="C26" s="117"/>
-      <c r="D26" s="118"/>
-      <c r="E26" s="118"/>
-      <c r="F26" s="118"/>
-      <c r="G26" s="118"/>
-      <c r="H26" s="200"/>
-      <c r="I26" s="200"/>
-      <c r="J26" s="119"/>
-      <c r="K26" s="118"/>
-      <c r="L26" s="57"/>
+      <c r="B26" s="115"/>
+      <c r="C26" s="116"/>
+      <c r="D26" s="117"/>
+      <c r="E26" s="117"/>
+      <c r="F26" s="117"/>
+      <c r="G26" s="117"/>
+      <c r="H26" s="199"/>
+      <c r="I26" s="199"/>
+      <c r="J26" s="118"/>
+      <c r="K26" s="117"/>
+      <c r="L26" s="56"/>
     </row>
     <row r="27" spans="1:12" s="6" customFormat="1" ht="16.2">
-      <c r="A27" s="120" t="s">
+      <c r="A27" s="119" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="121"/>
-      <c r="C27" s="122"/>
-      <c r="D27" s="123"/>
-      <c r="E27" s="123"/>
-      <c r="F27" s="123"/>
-      <c r="G27" s="123"/>
-      <c r="H27" s="124"/>
-      <c r="I27" s="123"/>
-      <c r="J27" s="123"/>
-      <c r="K27" s="123"/>
-      <c r="L27" s="57"/>
+      <c r="B27" s="120"/>
+      <c r="C27" s="121"/>
+      <c r="D27" s="122"/>
+      <c r="E27" s="122"/>
+      <c r="F27" s="122"/>
+      <c r="G27" s="122"/>
+      <c r="H27" s="123"/>
+      <c r="I27" s="122"/>
+      <c r="J27" s="122"/>
+      <c r="K27" s="122"/>
+      <c r="L27" s="56"/>
     </row>
     <row r="28" spans="1:12" s="9" customFormat="1" ht="16.2">
       <c r="A28" s="13"/>
@@ -6756,87 +6751,87 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="19.8"/>
   <cols>
-    <col min="1" max="1" width="11.296875" style="154" customWidth="1"/>
-    <col min="2" max="2" width="52" style="125" customWidth="1"/>
-    <col min="3" max="3" width="26.796875" style="125" customWidth="1"/>
-    <col min="4" max="4" width="10.296875" style="125" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5" style="125" customWidth="1"/>
-    <col min="7" max="16384" width="8.69921875" style="125"/>
+    <col min="1" max="1" width="11.296875" style="153" customWidth="1"/>
+    <col min="2" max="2" width="52" style="124" customWidth="1"/>
+    <col min="3" max="3" width="26.796875" style="124" customWidth="1"/>
+    <col min="4" max="4" width="10.296875" style="124" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="124" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5" style="124" customWidth="1"/>
+    <col min="7" max="16384" width="8.69921875" style="124"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.2">
-      <c r="A1" s="224" t="s">
+      <c r="A1" s="223" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="224"/>
-      <c r="C1" s="224"/>
+      <c r="B1" s="223"/>
+      <c r="C1" s="223"/>
     </row>
     <row r="2" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A2" s="126"/>
-      <c r="B2" s="127" t="s">
+      <c r="A2" s="125"/>
+      <c r="B2" s="126" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="126"/>
+      <c r="C2" s="125"/>
     </row>
     <row r="3" spans="1:6" ht="20.399999999999999" thickBot="1">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="127" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="129"/>
-      <c r="C3" s="130" t="s">
+      <c r="B3" s="128"/>
+      <c r="C3" s="129" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="20.399999999999999" thickBot="1">
-      <c r="A4" s="228" t="s">
+      <c r="A4" s="227" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="131" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="132" t="s">
+      <c r="B4" s="130" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="131" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="133"/>
+      <c r="D4" s="132"/>
     </row>
     <row r="5" spans="1:6" ht="20.399999999999999">
-      <c r="A5" s="229"/>
+      <c r="A5" s="228"/>
       <c r="B5" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="134"/>
-      <c r="D5" s="135"/>
+      <c r="C5" s="133"/>
+      <c r="D5" s="134"/>
       <c r="E5" s="47"/>
-      <c r="F5" s="136"/>
+      <c r="F5" s="135"/>
     </row>
     <row r="6" spans="1:6" ht="20.399999999999999">
-      <c r="A6" s="229"/>
+      <c r="A6" s="228"/>
       <c r="B6" s="41" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="48"/>
-      <c r="D6" s="135"/>
+      <c r="D6" s="134"/>
     </row>
     <row r="7" spans="1:6" ht="20.399999999999999">
-      <c r="A7" s="229"/>
+      <c r="A7" s="228"/>
       <c r="B7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="137"/>
-      <c r="D7" s="135"/>
-      <c r="E7" s="138"/>
+      <c r="C7" s="136"/>
+      <c r="D7" s="134"/>
+      <c r="E7" s="137"/>
     </row>
     <row r="8" spans="1:6" ht="20.399999999999999">
-      <c r="A8" s="229"/>
+      <c r="A8" s="228"/>
       <c r="B8" s="41" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="48"/>
-      <c r="D8" s="135"/>
+      <c r="D8" s="134"/>
     </row>
     <row r="9" spans="1:6" ht="21.6" thickBot="1">
-      <c r="A9" s="229"/>
+      <c r="A9" s="228"/>
       <c r="B9" s="34" t="s">
         <v>12</v>
       </c>
@@ -6844,56 +6839,56 @@
         <f>SUM(C5:C8)</f>
         <v>0</v>
       </c>
-      <c r="D9" s="135"/>
-      <c r="E9" s="139"/>
+      <c r="D9" s="134"/>
+      <c r="E9" s="138"/>
     </row>
     <row r="10" spans="1:6" ht="16.8" thickBot="1">
-      <c r="A10" s="229"/>
-      <c r="B10" s="140" t="s">
+      <c r="A10" s="228"/>
+      <c r="B10" s="139" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="141" t="s">
+      <c r="C10" s="140" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.2">
-      <c r="A11" s="229"/>
+      <c r="A11" s="228"/>
       <c r="B11" s="42" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="43"/>
     </row>
     <row r="12" spans="1:6" ht="20.399999999999999">
-      <c r="A12" s="229"/>
+      <c r="A12" s="228"/>
       <c r="B12" s="44" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="45"/>
     </row>
     <row r="13" spans="1:6" ht="21.6" thickBot="1">
-      <c r="A13" s="229"/>
+      <c r="A13" s="228"/>
       <c r="B13" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="142">
+      <c r="C13" s="141">
         <f>SUM(C11:C12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" customHeight="1" thickBot="1">
-      <c r="A14" s="230"/>
-      <c r="B14" s="131" t="s">
+      <c r="A14" s="229"/>
+      <c r="B14" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="143">
+      <c r="C14" s="142">
         <f>C9+C13</f>
         <v>0</v>
       </c>
       <c r="E14" s="47"/>
-      <c r="F14" s="139"/>
+      <c r="F14" s="138"/>
     </row>
     <row r="15" spans="1:6" ht="21.6" thickBot="1">
-      <c r="A15" s="231" t="s">
+      <c r="A15" s="230" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="32" t="s">
@@ -6903,43 +6898,43 @@
       <c r="E15" s="47"/>
     </row>
     <row r="16" spans="1:6" ht="21.6" thickBot="1">
-      <c r="A16" s="232"/>
-      <c r="B16" s="144" t="s">
+      <c r="A16" s="231"/>
+      <c r="B16" s="143" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="145"/>
-      <c r="E16" s="146"/>
+      <c r="C16" s="144"/>
+      <c r="E16" s="145"/>
     </row>
     <row r="17" spans="1:6" ht="21">
-      <c r="A17" s="232"/>
+      <c r="A17" s="231"/>
       <c r="B17" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="147"/>
+      <c r="C17" s="146"/>
     </row>
     <row r="18" spans="1:6" ht="16.2">
-      <c r="A18" s="232"/>
+      <c r="A18" s="231"/>
       <c r="B18" s="36" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="37"/>
     </row>
     <row r="19" spans="1:6" ht="16.2">
-      <c r="A19" s="232"/>
+      <c r="A19" s="231"/>
       <c r="B19" s="36" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="37"/>
     </row>
     <row r="20" spans="1:6" ht="16.2">
-      <c r="A20" s="232"/>
+      <c r="A20" s="231"/>
       <c r="B20" s="36" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="37"/>
     </row>
     <row r="21" spans="1:6" ht="21.6" thickBot="1">
-      <c r="A21" s="232"/>
+      <c r="A21" s="231"/>
       <c r="B21" s="34" t="s">
         <v>4</v>
       </c>
@@ -6947,80 +6942,80 @@
         <f>SUM(C17:C20)</f>
         <v>0</v>
       </c>
-      <c r="D21" s="135"/>
-      <c r="E21" s="139"/>
+      <c r="D21" s="134"/>
+      <c r="E21" s="138"/>
     </row>
     <row r="22" spans="1:6" ht="21.6" thickBot="1">
-      <c r="A22" s="232"/>
-      <c r="B22" s="144" t="s">
+      <c r="A22" s="231"/>
+      <c r="B22" s="143" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="145"/>
+      <c r="C22" s="144"/>
       <c r="E22" s="47"/>
     </row>
     <row r="23" spans="1:6" ht="16.2">
-      <c r="A23" s="232"/>
+      <c r="A23" s="231"/>
       <c r="B23" s="38" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="39"/>
     </row>
     <row r="24" spans="1:6" ht="20.399999999999999">
-      <c r="A24" s="232"/>
+      <c r="A24" s="231"/>
       <c r="B24" s="44" t="s">
         <v>24</v>
       </c>
       <c r="C24" s="46"/>
     </row>
     <row r="25" spans="1:6" ht="21.6" thickBot="1">
-      <c r="A25" s="148"/>
+      <c r="A25" s="147"/>
       <c r="B25" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="142">
+      <c r="C25" s="141">
         <f>SUM(C23:C24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" customHeight="1" thickBot="1">
-      <c r="A26" s="149"/>
-      <c r="B26" s="131" t="s">
+      <c r="A26" s="148"/>
+      <c r="B26" s="130" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="143">
+      <c r="C26" s="142">
         <f>C21+C25</f>
         <v>0</v>
       </c>
       <c r="E26" s="47"/>
-      <c r="F26" s="139"/>
+      <c r="F26" s="138"/>
     </row>
     <row r="27" spans="1:6" ht="42" customHeight="1" thickBot="1">
-      <c r="A27" s="226" t="s">
+      <c r="A27" s="225" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="227"/>
-      <c r="C27" s="150">
+      <c r="B27" s="226"/>
+      <c r="C27" s="149">
         <f>C14+C26</f>
         <v>0</v>
       </c>
-      <c r="D27" s="151" t="s">
+      <c r="D27" s="150" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="152"/>
-      <c r="F27" s="153">
+      <c r="E27" s="151"/>
+      <c r="F27" s="152">
         <v>9.999847412109375E-2</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="154" t="s">
+      <c r="A28" s="153" t="s">
         <v>74</v>
       </c>
       <c r="B28" s="5"/>
-      <c r="C28" s="155"/>
-      <c r="D28" s="156" t="s">
+      <c r="C28" s="154"/>
+      <c r="D28" s="155" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="157"/>
+      <c r="E28" s="156"/>
     </row>
     <row r="29" spans="1:6" ht="57.75" customHeight="1">
       <c r="B29" s="5"/>
@@ -7028,49 +7023,49 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="158" customFormat="1" ht="17.399999999999999">
-      <c r="A30" s="225" t="s">
+    <row r="30" spans="1:6" s="157" customFormat="1" ht="17.399999999999999">
+      <c r="A30" s="224" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="225"/>
-      <c r="C30" s="225"/>
+      <c r="B30" s="224"/>
+      <c r="C30" s="224"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="C31" s="125" t="s">
+      <c r="C31" s="124" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="C32" s="125" t="s">
+      <c r="C32" s="124" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="33" spans="3:4">
-      <c r="C33" s="159"/>
-      <c r="D33" s="160"/>
+      <c r="C33" s="158"/>
+      <c r="D33" s="159"/>
     </row>
     <row r="34" spans="3:4">
-      <c r="C34" s="125" t="s">
+      <c r="C34" s="124" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="37" spans="3:4">
-      <c r="C37" s="125" t="s">
+      <c r="C37" s="124" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="39" spans="3:4">
-      <c r="C39" s="125" t="s">
+      <c r="C39" s="124" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="40" spans="3:4">
-      <c r="C40" s="125" t="s">
+      <c r="C40" s="124" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="41" spans="3:4">
-      <c r="C41" s="125" t="s">
+      <c r="C41" s="124" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7095,542 +7090,574 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:P27"/>
+  <dimension ref="A3:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="2" width="17.69921875" style="163" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.69921875" style="163" customWidth="1"/>
-    <col min="4" max="4" width="16.296875" style="163" customWidth="1"/>
-    <col min="5" max="7" width="13.09765625" style="163" customWidth="1"/>
-    <col min="8" max="8" width="17.5" style="163" customWidth="1"/>
-    <col min="9" max="9" width="22.69921875" style="163" customWidth="1"/>
-    <col min="10" max="10" width="17.69921875" style="163" customWidth="1"/>
-    <col min="11" max="11" width="14.69921875" style="163" customWidth="1"/>
-    <col min="12" max="12" width="13.59765625" style="163" customWidth="1"/>
-    <col min="13" max="13" width="13.3984375" style="163" customWidth="1"/>
-    <col min="14" max="14" width="15.296875" style="163" customWidth="1"/>
-    <col min="15" max="15" width="18.09765625" style="163" customWidth="1"/>
-    <col min="16" max="16" width="20.5" style="163" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.69921875" style="163"/>
+    <col min="1" max="2" width="17.69921875" style="162" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.69921875" style="162" customWidth="1"/>
+    <col min="4" max="4" width="16.296875" style="162" customWidth="1"/>
+    <col min="5" max="7" width="13.09765625" style="162" customWidth="1"/>
+    <col min="8" max="8" width="17.5" style="162" customWidth="1"/>
+    <col min="9" max="9" width="22.69921875" style="162" customWidth="1"/>
+    <col min="10" max="10" width="17.69921875" style="162" customWidth="1"/>
+    <col min="11" max="11" width="14.69921875" style="162" customWidth="1"/>
+    <col min="12" max="12" width="13.59765625" style="162" customWidth="1"/>
+    <col min="13" max="13" width="13.3984375" style="162" customWidth="1"/>
+    <col min="14" max="14" width="15.296875" style="162" customWidth="1"/>
+    <col min="15" max="15" width="18.09765625" style="162" customWidth="1"/>
+    <col min="16" max="16" width="20.5" style="162" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.296875" style="162" customWidth="1"/>
+    <col min="18" max="16384" width="8.69921875" style="162"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" ht="16.8" thickBot="1">
-      <c r="A3" s="53"/>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53" t="s">
+    <row r="3" spans="1:17" ht="16.8" thickBot="1">
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="161"/>
-      <c r="J3" s="162"/>
-      <c r="K3" s="162"/>
-      <c r="L3" s="162"/>
-      <c r="M3" s="162"/>
-      <c r="N3" s="162"/>
-      <c r="O3" s="162"/>
-      <c r="P3" s="162"/>
-    </row>
-    <row r="4" spans="1:16" s="168" customFormat="1" ht="33" thickTop="1">
-      <c r="A4" s="164" t="s">
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="160"/>
+      <c r="J3" s="161"/>
+      <c r="K3" s="161"/>
+      <c r="L3" s="161"/>
+      <c r="M3" s="161"/>
+      <c r="N3" s="161"/>
+      <c r="O3" s="161"/>
+      <c r="P3" s="161"/>
+    </row>
+    <row r="4" spans="1:17" s="167" customFormat="1" ht="33" thickTop="1">
+      <c r="A4" s="163" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="165" t="s">
+      <c r="B4" s="164" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="165">
+      <c r="C4" s="164">
         <v>1</v>
       </c>
-      <c r="D4" s="165">
+      <c r="D4" s="164">
         <v>2</v>
       </c>
-      <c r="E4" s="165">
+      <c r="E4" s="164">
         <v>3</v>
       </c>
-      <c r="F4" s="165">
+      <c r="F4" s="164">
         <v>4</v>
       </c>
-      <c r="G4" s="165">
+      <c r="G4" s="164">
         <v>5</v>
       </c>
-      <c r="H4" s="165" t="s">
+      <c r="H4" s="164" t="s">
         <v>101</v>
       </c>
-      <c r="I4" s="166" t="s">
+      <c r="I4" s="165" t="s">
         <v>76</v>
       </c>
-      <c r="J4" s="195" t="s">
+      <c r="J4" s="194" t="s">
         <v>86</v>
       </c>
-      <c r="K4" s="196" t="s">
+      <c r="K4" s="235" t="s">
         <v>87</v>
       </c>
-      <c r="L4" s="51" t="s">
+      <c r="L4" s="235" t="s">
         <v>88</v>
       </c>
-      <c r="M4" s="52" t="s">
+      <c r="M4" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="N4" s="52" t="s">
+      <c r="N4" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="O4" s="167" t="s">
+      <c r="O4" s="166" t="s">
         <v>76</v>
       </c>
       <c r="P4" s="50" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="233" t="s">
+      <c r="Q4" s="234" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="232" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="165" t="s">
+      <c r="B5" s="164" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="169"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="169">
+      <c r="C5" s="168"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="168">
         <f t="shared" ref="I5:I10" si="0">SUM(C5:H5)</f>
         <v>0</v>
       </c>
-      <c r="J5" s="192"/>
-      <c r="K5" s="189"/>
-      <c r="L5" s="191"/>
-      <c r="M5" s="191"/>
-      <c r="N5" s="191"/>
-      <c r="O5" s="187">
+      <c r="J5" s="191"/>
+      <c r="K5" s="188"/>
+      <c r="L5" s="190"/>
+      <c r="M5" s="190"/>
+      <c r="N5" s="190"/>
+      <c r="O5" s="186">
         <f t="shared" ref="O5:O9" si="1">SUM(J5:N5)</f>
         <v>0</v>
       </c>
-      <c r="P5" s="199"/>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="234"/>
-      <c r="B6" s="165" t="s">
+      <c r="P5" s="197"/>
+      <c r="Q5" s="175">
+        <f>I5-P5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="233"/>
+      <c r="B6" s="164" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="169"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="169">
+      <c r="C6" s="168"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="168">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J6" s="193"/>
-      <c r="K6" s="197"/>
-      <c r="L6" s="190"/>
-      <c r="M6" s="190"/>
-      <c r="N6" s="190"/>
-      <c r="O6" s="187">
+      <c r="J6" s="192"/>
+      <c r="K6" s="195"/>
+      <c r="L6" s="189"/>
+      <c r="M6" s="189"/>
+      <c r="N6" s="189"/>
+      <c r="O6" s="186">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P6" s="199"/>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="165" t="s">
+      <c r="P6" s="197"/>
+      <c r="Q6" s="175">
+        <f t="shared" ref="Q6:Q11" si="2">I6-P6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="164" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="165"/>
-      <c r="C7" s="169"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="170">
+      <c r="B7" s="164"/>
+      <c r="C7" s="168"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="169">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J7" s="192"/>
-      <c r="K7" s="189"/>
-      <c r="L7" s="191"/>
-      <c r="M7" s="191"/>
-      <c r="N7" s="191"/>
-      <c r="O7" s="187">
+      <c r="J7" s="191"/>
+      <c r="K7" s="188"/>
+      <c r="L7" s="190"/>
+      <c r="M7" s="190"/>
+      <c r="N7" s="190"/>
+      <c r="O7" s="186">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P7" s="199"/>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="233" t="s">
+      <c r="P7" s="197"/>
+      <c r="Q7" s="175">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="232" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="165" t="s">
+      <c r="B8" s="164" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="169"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="169">
+      <c r="C8" s="168"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="168">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J8" s="192"/>
-      <c r="K8" s="189"/>
-      <c r="L8" s="191"/>
-      <c r="M8" s="191"/>
-      <c r="N8" s="191"/>
-      <c r="O8" s="187">
+      <c r="J8" s="191"/>
+      <c r="K8" s="188"/>
+      <c r="L8" s="190"/>
+      <c r="M8" s="190"/>
+      <c r="N8" s="190"/>
+      <c r="O8" s="186">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P8" s="199"/>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="234"/>
-      <c r="B9" s="165" t="s">
+      <c r="P8" s="197"/>
+      <c r="Q8" s="175">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="233"/>
+      <c r="B9" s="164" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="169"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="169">
+      <c r="C9" s="168"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="168">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J9" s="193"/>
-      <c r="K9" s="197"/>
-      <c r="L9" s="190"/>
-      <c r="M9" s="190"/>
-      <c r="N9" s="190"/>
-      <c r="O9" s="187">
+      <c r="J9" s="192"/>
+      <c r="K9" s="195"/>
+      <c r="L9" s="189"/>
+      <c r="M9" s="189"/>
+      <c r="N9" s="189"/>
+      <c r="O9" s="186">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P9" s="199"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="165" t="s">
+      <c r="P9" s="197"/>
+      <c r="Q9" s="175">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="164" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="165"/>
-      <c r="C10" s="169"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="169">
+      <c r="B10" s="164"/>
+      <c r="C10" s="168"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="168">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J10" s="193"/>
-      <c r="K10" s="189"/>
-      <c r="L10" s="191"/>
-      <c r="M10" s="191"/>
-      <c r="N10" s="191"/>
-      <c r="O10" s="188"/>
-      <c r="P10" s="199"/>
-    </row>
-    <row r="11" spans="1:16" ht="16.8" thickBot="1">
-      <c r="A11" s="171" t="s">
+      <c r="J10" s="192"/>
+      <c r="K10" s="188"/>
+      <c r="L10" s="190"/>
+      <c r="M10" s="190"/>
+      <c r="N10" s="190"/>
+      <c r="O10" s="187"/>
+      <c r="P10" s="197"/>
+      <c r="Q10" s="175">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="16.8" thickBot="1">
+      <c r="A11" s="170" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="171"/>
-      <c r="C11" s="169">
-        <f t="shared" ref="C11:J11" si="2">SUM(C5:C10)</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="169">
+      <c r="B11" s="170"/>
+      <c r="C11" s="168">
+        <f t="shared" ref="C11:J11" si="3">SUM(C5:C10)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="168">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="168">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="168">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="168">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="168">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="168">
+        <f>SUM(I5:I10)</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="193">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="196">
+        <f t="shared" ref="K11:N11" si="4">SUM(K5:K10)</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="171">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="171">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="171">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="172">
+        <f>SUM(O5:O10)</f>
+        <v>0</v>
+      </c>
+      <c r="P11" s="173">
+        <f>SUM(P5:P10)</f>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="175">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E11" s="169">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="169">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="169">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="169">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="169">
-        <f>SUM(I5:I10)</f>
-        <v>0</v>
-      </c>
-      <c r="J11" s="194">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K11" s="198">
-        <f t="shared" ref="K11:N11" si="3">SUM(K5:K10)</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="172">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M11" s="172">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="172">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="173">
-        <f>SUM(O5:O10)</f>
-        <v>0</v>
-      </c>
-      <c r="P11" s="174">
-        <f>SUM(P5:P10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="16.8" thickTop="1">
-      <c r="A12" s="163" t="s">
+    </row>
+    <row r="12" spans="1:17" ht="16.8" thickTop="1">
+      <c r="A12" s="162" t="s">
         <v>103</v>
       </c>
-      <c r="D12" s="163" t="s">
+      <c r="D12" s="162" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="163" t="s">
+    <row r="13" spans="1:17">
+      <c r="A13" s="162" t="s">
         <v>91</v>
       </c>
-      <c r="H13" s="163" t="s">
+      <c r="H13" s="162" t="s">
         <v>97</v>
       </c>
-      <c r="N13" s="175" t="s">
+      <c r="N13" s="174" t="s">
         <v>100</v>
       </c>
-      <c r="O13" s="176">
+      <c r="O13" s="175">
         <f>P13-O11</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="163" t="s">
+    <row r="14" spans="1:17">
+      <c r="A14" s="162" t="s">
         <v>92</v>
       </c>
-      <c r="G14" s="177" t="s">
+      <c r="G14" s="176" t="s">
         <v>98</v>
       </c>
-      <c r="H14" s="175" t="s">
+      <c r="H14" s="174" t="s">
         <v>99</v>
       </c>
-      <c r="I14" s="175"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="163" t="s">
+      <c r="I14" s="174"/>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="162" t="s">
         <v>93</v>
       </c>
-      <c r="B15" s="186"/>
-      <c r="C15" s="235"/>
-      <c r="I15" s="176">
+      <c r="B15" s="185"/>
+      <c r="C15" s="198"/>
+      <c r="I15" s="175">
         <f>SUM(I8:I9)-I14</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="163" t="s">
+    <row r="16" spans="1:17">
+      <c r="A16" s="162" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="163" t="s">
+      <c r="A17" s="162" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="176"/>
-      <c r="C17" s="176">
+      <c r="B17" s="175"/>
+      <c r="C17" s="175">
         <f>H21</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="178" t="s">
+      <c r="A19" s="177" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="179"/>
-      <c r="C19" s="180"/>
-      <c r="D19" s="53" t="s">
+      <c r="B19" s="178"/>
+      <c r="C19" s="179"/>
+      <c r="D19" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="161"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="160"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="181" t="s">
+      <c r="A20" s="180" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="182" t="s">
+      <c r="B20" s="181" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="165">
+      <c r="C20" s="164">
         <v>1</v>
       </c>
-      <c r="D20" s="165">
+      <c r="D20" s="164">
         <v>2</v>
       </c>
-      <c r="E20" s="165">
+      <c r="E20" s="164">
         <v>3</v>
       </c>
-      <c r="F20" s="165">
+      <c r="F20" s="164">
         <v>5</v>
       </c>
-      <c r="G20" s="165" t="s">
+      <c r="G20" s="164" t="s">
         <v>101</v>
       </c>
-      <c r="H20" s="165" t="s">
+      <c r="H20" s="164" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="233" t="s">
+      <c r="A21" s="232" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="165" t="s">
+      <c r="B21" s="164" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="171"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55">
+      <c r="C21" s="170"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54">
         <f>SUM(C21:F21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="234"/>
-      <c r="B22" s="165" t="s">
+      <c r="A22" s="233"/>
+      <c r="B22" s="164" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="171"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55">
-        <f t="shared" ref="H22:H27" si="4">SUM(C22:F22)</f>
+      <c r="C22" s="170"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54">
+        <f t="shared" ref="H22:H27" si="5">SUM(C22:F22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="165" t="s">
+      <c r="A23" s="164" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="165" t="s">
+      <c r="B23" s="164" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="171"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="55">
-        <f t="shared" si="4"/>
+      <c r="C23" s="170"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="233" t="s">
+      <c r="A24" s="232" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="165" t="s">
+      <c r="B24" s="164" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="171"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55">
-        <f t="shared" si="4"/>
+      <c r="C24" s="170"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="234"/>
-      <c r="B25" s="165" t="s">
+      <c r="A25" s="233"/>
+      <c r="B25" s="164" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="171"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55">
-        <f t="shared" si="4"/>
+      <c r="C25" s="170"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="54">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="183" t="s">
+      <c r="A26" s="182" t="s">
         <v>81</v>
       </c>
-      <c r="B26" s="183" t="s">
+      <c r="B26" s="182" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="171"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55">
-        <f t="shared" si="4"/>
+      <c r="C26" s="170"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="178" t="s">
+      <c r="A27" s="177" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="179"/>
-      <c r="C27" s="55">
+      <c r="B27" s="178"/>
+      <c r="C27" s="54">
         <f>SUM(C21:C25)</f>
         <v>0</v>
       </c>
-      <c r="D27" s="55">
-        <f t="shared" ref="D27:E27" si="5">SUM(D21:D25)</f>
-        <v>0</v>
-      </c>
-      <c r="E27" s="55">
+      <c r="D27" s="54">
+        <f t="shared" ref="D27:E27" si="6">SUM(D21:D25)</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="54">
+        <f>SUM(F21:F25)</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="55">
-        <f>SUM(F21:F25)</f>
-        <v>0</v>
-      </c>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto-committed on 2023/10/11 週三 11:47:55.17
</commit_message>
<xml_diff>
--- a/Program/Other/LM042_底稿_RBC表_會計部_共三份.xlsx
+++ b/Program/Other/LM042_底稿_RBC表_會計部_共三份.xlsx
@@ -956,10 +956,6 @@
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <t>差異數</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
     <t>(空白)</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -981,6 +977,10 @@
   </si>
   <si>
     <t>淨額</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.5% 差異數</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
@@ -3987,6 +3987,12 @@
     <xf numFmtId="178" fontId="80" fillId="0" borderId="0" xfId="86" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4091,12 +4097,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="80" fillId="0" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="188">
@@ -5850,85 +5850,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="33">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="202" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="200"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="200"/>
-      <c r="F1" s="200"/>
-      <c r="G1" s="200"/>
-      <c r="H1" s="200"/>
-      <c r="I1" s="200"/>
-      <c r="J1" s="200"/>
+      <c r="B1" s="202"/>
+      <c r="C1" s="202"/>
+      <c r="D1" s="202"/>
+      <c r="E1" s="202"/>
+      <c r="F1" s="202"/>
+      <c r="G1" s="202"/>
+      <c r="H1" s="202"/>
+      <c r="I1" s="202"/>
+      <c r="J1" s="202"/>
       <c r="K1" s="55"/>
       <c r="L1" s="56"/>
     </row>
     <row r="2" spans="1:12" ht="16.2">
-      <c r="A2" s="214" t="s">
+      <c r="A2" s="216" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="214"/>
-      <c r="C2" s="214"/>
-      <c r="D2" s="214"/>
-      <c r="E2" s="214"/>
-      <c r="F2" s="214"/>
-      <c r="G2" s="214"/>
-      <c r="H2" s="214"/>
-      <c r="I2" s="214"/>
-      <c r="J2" s="214"/>
+      <c r="B2" s="216"/>
+      <c r="C2" s="216"/>
+      <c r="D2" s="216"/>
+      <c r="E2" s="216"/>
+      <c r="F2" s="216"/>
+      <c r="G2" s="216"/>
+      <c r="H2" s="216"/>
+      <c r="I2" s="216"/>
+      <c r="J2" s="216"/>
       <c r="K2" s="57" t="s">
         <v>26</v>
       </c>
       <c r="L2" s="56"/>
     </row>
     <row r="3" spans="1:12" ht="16.2" thickBot="1">
-      <c r="A3" s="215"/>
-      <c r="B3" s="215"/>
-      <c r="C3" s="215"/>
-      <c r="D3" s="215"/>
-      <c r="E3" s="215"/>
-      <c r="F3" s="215"/>
-      <c r="G3" s="215"/>
-      <c r="H3" s="215"/>
-      <c r="I3" s="215"/>
-      <c r="J3" s="215"/>
+      <c r="A3" s="217"/>
+      <c r="B3" s="217"/>
+      <c r="C3" s="217"/>
+      <c r="D3" s="217"/>
+      <c r="E3" s="217"/>
+      <c r="F3" s="217"/>
+      <c r="G3" s="217"/>
+      <c r="H3" s="217"/>
+      <c r="I3" s="217"/>
+      <c r="J3" s="217"/>
       <c r="K3" s="58" t="s">
         <v>31</v>
       </c>
       <c r="L3" s="56"/>
     </row>
     <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A4" s="201" t="s">
+      <c r="A4" s="203" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="202"/>
-      <c r="C4" s="205" t="s">
+      <c r="B4" s="204"/>
+      <c r="C4" s="207" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="207" t="s">
+      <c r="D4" s="209" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="207"/>
-      <c r="F4" s="210" t="s">
+      <c r="E4" s="209"/>
+      <c r="F4" s="212" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="211"/>
-      <c r="H4" s="212" t="s">
+      <c r="G4" s="213"/>
+      <c r="H4" s="214" t="s">
         <v>71</v>
       </c>
-      <c r="I4" s="213"/>
-      <c r="J4" s="208" t="s">
+      <c r="I4" s="215"/>
+      <c r="J4" s="210" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="209"/>
+      <c r="K4" s="211"/>
       <c r="L4" s="56"/>
     </row>
     <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1" thickTop="1">
-      <c r="A5" s="203"/>
-      <c r="B5" s="204"/>
-      <c r="C5" s="206"/>
+      <c r="A5" s="205"/>
+      <c r="B5" s="206"/>
+      <c r="C5" s="208"/>
       <c r="D5" s="59" t="s">
         <v>27</v>
       </c>
@@ -5956,7 +5956,7 @@
       <c r="L5" s="56"/>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
-      <c r="A6" s="216" t="s">
+      <c r="A6" s="218" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="66" t="s">
@@ -5974,7 +5974,7 @@
       <c r="L6" s="56"/>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
-      <c r="A7" s="217"/>
+      <c r="A7" s="219"/>
       <c r="B7" s="73" t="s">
         <v>36</v>
       </c>
@@ -6010,7 +6010,7 @@
       <c r="L7" s="56"/>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1">
-      <c r="A8" s="217"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="73" t="s">
         <v>37</v>
       </c>
@@ -6046,7 +6046,7 @@
       <c r="L8" s="56"/>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1">
-      <c r="A9" s="217"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="73" t="s">
         <v>38</v>
       </c>
@@ -6082,7 +6082,7 @@
       <c r="L9" s="56"/>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1">
-      <c r="A10" s="217"/>
+      <c r="A10" s="219"/>
       <c r="B10" s="73" t="s">
         <v>39</v>
       </c>
@@ -6118,7 +6118,7 @@
       <c r="L10" s="56"/>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1">
-      <c r="A11" s="217"/>
+      <c r="A11" s="219"/>
       <c r="B11" s="81" t="s">
         <v>40</v>
       </c>
@@ -6158,7 +6158,7 @@
       <c r="L11" s="56"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
-      <c r="A12" s="217"/>
+      <c r="A12" s="219"/>
       <c r="B12" s="66" t="s">
         <v>41</v>
       </c>
@@ -6174,7 +6174,7 @@
       <c r="L12" s="56"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
-      <c r="A13" s="217"/>
+      <c r="A13" s="219"/>
       <c r="B13" s="90" t="s">
         <v>42</v>
       </c>
@@ -6202,7 +6202,7 @@
       <c r="L13" s="56"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
-      <c r="A14" s="217"/>
+      <c r="A14" s="219"/>
       <c r="B14" s="90" t="s">
         <v>43</v>
       </c>
@@ -6238,7 +6238,7 @@
       <c r="L14" s="56"/>
     </row>
     <row r="15" spans="1:12" ht="28.95" customHeight="1">
-      <c r="A15" s="217"/>
+      <c r="A15" s="219"/>
       <c r="B15" s="81" t="s">
         <v>44</v>
       </c>
@@ -6278,7 +6278,7 @@
       <c r="L15" s="56"/>
     </row>
     <row r="16" spans="1:12" ht="34.5" customHeight="1" thickBot="1">
-      <c r="A16" s="218"/>
+      <c r="A16" s="220"/>
       <c r="B16" s="96" t="s">
         <v>45</v>
       </c>
@@ -6318,7 +6318,7 @@
       <c r="L16" s="100"/>
     </row>
     <row r="17" spans="1:12" ht="33.75" customHeight="1" thickTop="1">
-      <c r="A17" s="219" t="s">
+      <c r="A17" s="221" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="101" t="s">
@@ -6360,7 +6360,7 @@
       <c r="L17" s="105"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
-      <c r="A18" s="220"/>
+      <c r="A18" s="222"/>
       <c r="B18" s="66" t="s">
         <v>35</v>
       </c>
@@ -6376,7 +6376,7 @@
       <c r="L18" s="56"/>
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
-      <c r="A19" s="220"/>
+      <c r="A19" s="222"/>
       <c r="B19" s="90" t="s">
         <v>47</v>
       </c>
@@ -6412,7 +6412,7 @@
       <c r="L19" s="56"/>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1">
-      <c r="A20" s="220"/>
+      <c r="A20" s="222"/>
       <c r="B20" s="81" t="s">
         <v>48</v>
       </c>
@@ -6452,7 +6452,7 @@
       <c r="L20" s="56"/>
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
-      <c r="A21" s="220"/>
+      <c r="A21" s="222"/>
       <c r="B21" s="66" t="s">
         <v>41</v>
       </c>
@@ -6468,7 +6468,7 @@
       <c r="L21" s="56"/>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
-      <c r="A22" s="220"/>
+      <c r="A22" s="222"/>
       <c r="B22" s="90" t="s">
         <v>42</v>
       </c>
@@ -6502,7 +6502,7 @@
       <c r="L22" s="56"/>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
-      <c r="A23" s="220"/>
+      <c r="A23" s="222"/>
       <c r="B23" s="90" t="s">
         <v>43</v>
       </c>
@@ -6578,8 +6578,8 @@
       <c r="L24" s="56"/>
     </row>
     <row r="25" spans="1:12" ht="35.1" customHeight="1" thickBot="1">
-      <c r="A25" s="221"/>
-      <c r="B25" s="222"/>
+      <c r="A25" s="223"/>
+      <c r="B25" s="224"/>
       <c r="C25" s="113"/>
       <c r="D25" s="114">
         <f>D16+D17</f>
@@ -6625,8 +6625,8 @@
       <c r="E26" s="117"/>
       <c r="F26" s="117"/>
       <c r="G26" s="117"/>
-      <c r="H26" s="199"/>
-      <c r="I26" s="199"/>
+      <c r="H26" s="201"/>
+      <c r="I26" s="201"/>
       <c r="J26" s="118"/>
       <c r="K26" s="117"/>
       <c r="L26" s="56"/>
@@ -6761,11 +6761,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.2">
-      <c r="A1" s="223" t="s">
+      <c r="A1" s="225" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="223"/>
-      <c r="C1" s="223"/>
+      <c r="B1" s="225"/>
+      <c r="C1" s="225"/>
     </row>
     <row r="2" spans="1:6" ht="26.25" customHeight="1">
       <c r="A2" s="125"/>
@@ -6784,7 +6784,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="20.399999999999999" thickBot="1">
-      <c r="A4" s="227" t="s">
+      <c r="A4" s="229" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="130" t="s">
@@ -6796,7 +6796,7 @@
       <c r="D4" s="132"/>
     </row>
     <row r="5" spans="1:6" ht="20.399999999999999">
-      <c r="A5" s="228"/>
+      <c r="A5" s="230"/>
       <c r="B5" s="40" t="s">
         <v>8</v>
       </c>
@@ -6806,7 +6806,7 @@
       <c r="F5" s="135"/>
     </row>
     <row r="6" spans="1:6" ht="20.399999999999999">
-      <c r="A6" s="228"/>
+      <c r="A6" s="230"/>
       <c r="B6" s="41" t="s">
         <v>9</v>
       </c>
@@ -6814,7 +6814,7 @@
       <c r="D6" s="134"/>
     </row>
     <row r="7" spans="1:6" ht="20.399999999999999">
-      <c r="A7" s="228"/>
+      <c r="A7" s="230"/>
       <c r="B7" s="41" t="s">
         <v>10</v>
       </c>
@@ -6823,7 +6823,7 @@
       <c r="E7" s="137"/>
     </row>
     <row r="8" spans="1:6" ht="20.399999999999999">
-      <c r="A8" s="228"/>
+      <c r="A8" s="230"/>
       <c r="B8" s="41" t="s">
         <v>11</v>
       </c>
@@ -6831,7 +6831,7 @@
       <c r="D8" s="134"/>
     </row>
     <row r="9" spans="1:6" ht="21.6" thickBot="1">
-      <c r="A9" s="228"/>
+      <c r="A9" s="230"/>
       <c r="B9" s="34" t="s">
         <v>12</v>
       </c>
@@ -6843,7 +6843,7 @@
       <c r="E9" s="138"/>
     </row>
     <row r="10" spans="1:6" ht="16.8" thickBot="1">
-      <c r="A10" s="228"/>
+      <c r="A10" s="230"/>
       <c r="B10" s="139" t="s">
         <v>3</v>
       </c>
@@ -6852,21 +6852,21 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.2">
-      <c r="A11" s="228"/>
+      <c r="A11" s="230"/>
       <c r="B11" s="42" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="43"/>
     </row>
     <row r="12" spans="1:6" ht="20.399999999999999">
-      <c r="A12" s="228"/>
+      <c r="A12" s="230"/>
       <c r="B12" s="44" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="45"/>
     </row>
     <row r="13" spans="1:6" ht="21.6" thickBot="1">
-      <c r="A13" s="228"/>
+      <c r="A13" s="230"/>
       <c r="B13" s="34" t="s">
         <v>13</v>
       </c>
@@ -6876,7 +6876,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" customHeight="1" thickBot="1">
-      <c r="A14" s="229"/>
+      <c r="A14" s="231"/>
       <c r="B14" s="130" t="s">
         <v>14</v>
       </c>
@@ -6888,7 +6888,7 @@
       <c r="F14" s="138"/>
     </row>
     <row r="15" spans="1:6" ht="21.6" thickBot="1">
-      <c r="A15" s="230" t="s">
+      <c r="A15" s="232" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="32" t="s">
@@ -6898,7 +6898,7 @@
       <c r="E15" s="47"/>
     </row>
     <row r="16" spans="1:6" ht="21.6" thickBot="1">
-      <c r="A16" s="231"/>
+      <c r="A16" s="233"/>
       <c r="B16" s="143" t="s">
         <v>62</v>
       </c>
@@ -6906,35 +6906,35 @@
       <c r="E16" s="145"/>
     </row>
     <row r="17" spans="1:6" ht="21">
-      <c r="A17" s="231"/>
+      <c r="A17" s="233"/>
       <c r="B17" s="33" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="146"/>
     </row>
     <row r="18" spans="1:6" ht="16.2">
-      <c r="A18" s="231"/>
+      <c r="A18" s="233"/>
       <c r="B18" s="36" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="37"/>
     </row>
     <row r="19" spans="1:6" ht="16.2">
-      <c r="A19" s="231"/>
+      <c r="A19" s="233"/>
       <c r="B19" s="36" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="37"/>
     </row>
     <row r="20" spans="1:6" ht="16.2">
-      <c r="A20" s="231"/>
+      <c r="A20" s="233"/>
       <c r="B20" s="36" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="37"/>
     </row>
     <row r="21" spans="1:6" ht="21.6" thickBot="1">
-      <c r="A21" s="231"/>
+      <c r="A21" s="233"/>
       <c r="B21" s="34" t="s">
         <v>4</v>
       </c>
@@ -6946,7 +6946,7 @@
       <c r="E21" s="138"/>
     </row>
     <row r="22" spans="1:6" ht="21.6" thickBot="1">
-      <c r="A22" s="231"/>
+      <c r="A22" s="233"/>
       <c r="B22" s="143" t="s">
         <v>3</v>
       </c>
@@ -6954,14 +6954,14 @@
       <c r="E22" s="47"/>
     </row>
     <row r="23" spans="1:6" ht="16.2">
-      <c r="A23" s="231"/>
+      <c r="A23" s="233"/>
       <c r="B23" s="38" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="39"/>
     </row>
     <row r="24" spans="1:6" ht="20.399999999999999">
-      <c r="A24" s="231"/>
+      <c r="A24" s="233"/>
       <c r="B24" s="44" t="s">
         <v>24</v>
       </c>
@@ -6990,10 +6990,10 @@
       <c r="F26" s="138"/>
     </row>
     <row r="27" spans="1:6" ht="42" customHeight="1" thickBot="1">
-      <c r="A27" s="225" t="s">
+      <c r="A27" s="227" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="226"/>
+      <c r="B27" s="228"/>
       <c r="C27" s="149">
         <f>C14+C26</f>
         <v>0</v>
@@ -7024,11 +7024,11 @@
       </c>
     </row>
     <row r="30" spans="1:6" s="157" customFormat="1" ht="17.399999999999999">
-      <c r="A30" s="224" t="s">
+      <c r="A30" s="226" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="224"/>
-      <c r="C30" s="224"/>
+      <c r="B30" s="226"/>
+      <c r="C30" s="226"/>
     </row>
     <row r="31" spans="1:6">
       <c r="C31" s="124" t="s">
@@ -7093,7 +7093,7 @@
   <dimension ref="A3:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="16.2"/>
@@ -7158,7 +7158,7 @@
         <v>5</v>
       </c>
       <c r="H4" s="164" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I4" s="165" t="s">
         <v>76</v>
@@ -7166,10 +7166,10 @@
       <c r="J4" s="194" t="s">
         <v>86</v>
       </c>
-      <c r="K4" s="235" t="s">
+      <c r="K4" s="200" t="s">
         <v>87</v>
       </c>
-      <c r="L4" s="235" t="s">
+      <c r="L4" s="200" t="s">
         <v>88</v>
       </c>
       <c r="M4" s="51" t="s">
@@ -7184,12 +7184,12 @@
       <c r="P4" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="Q4" s="234" t="s">
-        <v>106</v>
+      <c r="Q4" s="199" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="232" t="s">
+      <c r="A5" s="234" t="s">
         <v>78</v>
       </c>
       <c r="B5" s="164" t="s">
@@ -7221,7 +7221,7 @@
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="233"/>
+      <c r="A6" s="235"/>
       <c r="B6" s="164" t="s">
         <v>85</v>
       </c>
@@ -7281,7 +7281,7 @@
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="232" t="s">
+      <c r="A8" s="234" t="s">
         <v>80</v>
       </c>
       <c r="B8" s="164" t="s">
@@ -7313,7 +7313,7 @@
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="233"/>
+      <c r="A9" s="235"/>
       <c r="B9" s="164" t="s">
         <v>85</v>
       </c>
@@ -7344,7 +7344,7 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="164" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" s="164"/>
       <c r="C10" s="168"/>
@@ -7437,10 +7437,10 @@
     </row>
     <row r="12" spans="1:17" ht="16.8" thickTop="1">
       <c r="A12" s="162" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="162" t="s">
         <v>103</v>
-      </c>
-      <c r="D12" s="162" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -7451,7 +7451,7 @@
         <v>97</v>
       </c>
       <c r="N13" s="174" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="O13" s="175">
         <f>P13-O11</f>
@@ -7488,7 +7488,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="162" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B17" s="175"/>
       <c r="C17" s="175">
@@ -7530,14 +7530,14 @@
         <v>5</v>
       </c>
       <c r="G20" s="164" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H20" s="164" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="232" t="s">
+      <c r="A21" s="234" t="s">
         <v>78</v>
       </c>
       <c r="B21" s="164" t="s">
@@ -7554,7 +7554,7 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="233"/>
+      <c r="A22" s="235"/>
       <c r="B22" s="164" t="s">
         <v>81</v>
       </c>
@@ -7586,7 +7586,7 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="232" t="s">
+      <c r="A24" s="234" t="s">
         <v>80</v>
       </c>
       <c r="B24" s="164" t="s">
@@ -7603,7 +7603,7 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="233"/>
+      <c r="A25" s="235"/>
       <c r="B25" s="164" t="s">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
Auto-committed on 2023/10/11 週三 16:22:31.96
</commit_message>
<xml_diff>
--- a/Program/Other/LM042_底稿_RBC表_會計部_共三份.xlsx
+++ b/Program/Other/LM042_底稿_RBC表_會計部_共三份.xlsx
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="109">
   <si>
     <t>一、非利害關係人放款</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -981,6 +981,14 @@
   </si>
   <si>
     <t>1.5% 差異數</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>科子細目淨額</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>差 額</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
@@ -7092,8 +7100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="16.2"/>
@@ -7469,6 +7477,9 @@
         <v>99</v>
       </c>
       <c r="I14" s="174"/>
+      <c r="N14" s="162" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="162" t="s">
@@ -7480,6 +7491,13 @@
         <f>SUM(I8:I9)-I14</f>
         <v>0</v>
       </c>
+      <c r="N15" s="167" t="s">
+        <v>108</v>
+      </c>
+      <c r="O15" s="175">
+        <f>O14-Q11</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="162" t="s">
@@ -7527,10 +7545,10 @@
         <v>3</v>
       </c>
       <c r="F20" s="164">
+        <v>4</v>
+      </c>
+      <c r="G20" s="164">
         <v>5</v>
-      </c>
-      <c r="G20" s="164" t="s">
-        <v>100</v>
       </c>
       <c r="H20" s="164" t="s">
         <v>76</v>
@@ -7549,7 +7567,7 @@
       <c r="F21" s="54"/>
       <c r="G21" s="54"/>
       <c r="H21" s="54">
-        <f>SUM(C21:F21)</f>
+        <f>SUM(C21:G21)</f>
         <v>0</v>
       </c>
     </row>
@@ -7564,7 +7582,7 @@
       <c r="F22" s="54"/>
       <c r="G22" s="54"/>
       <c r="H22" s="54">
-        <f t="shared" ref="H22:H27" si="5">SUM(C22:F22)</f>
+        <f t="shared" ref="H22:H27" si="5">SUM(C22:G22)</f>
         <v>0</v>
       </c>
     </row>
@@ -7655,7 +7673,10 @@
         <f>SUM(F21:F25)</f>
         <v>0</v>
       </c>
-      <c r="G27" s="54"/>
+      <c r="G27" s="54">
+        <f>SUM(G21:G25)</f>
+        <v>0</v>
+      </c>
       <c r="H27" s="54">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -7672,7 +7693,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="F11 C27:F27" formulaRange="1"/>
+    <ignoredError sqref="F11 C27:G27" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Auto-committed on 2023/10/12 週四 11:52:15.73
</commit_message>
<xml_diff>
--- a/Program/Other/LM042_底稿_RBC表_會計部_共三份.xlsx
+++ b/Program/Other/LM042_底稿_RBC表_會計部_共三份.xlsx
@@ -7100,8 +7100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="16.2"/>
@@ -7254,7 +7254,7 @@
       </c>
       <c r="P6" s="197"/>
       <c r="Q6" s="175">
-        <f t="shared" ref="Q6:Q11" si="2">I6-P6</f>
+        <f>I6-P6-O13</f>
         <v>0</v>
       </c>
     </row>
@@ -7284,7 +7284,7 @@
       </c>
       <c r="P7" s="197"/>
       <c r="Q7" s="175">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="Q6:Q11" si="2">I7-P7</f>
         <v>0</v>
       </c>
     </row>
@@ -7694,6 +7694,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="F11 C27:G27" formulaRange="1"/>
+    <ignoredError sqref="Q6" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>